<commit_message>
Spelling mistakes in categories
</commit_message>
<xml_diff>
--- a/GoogleOpenImages-allClasses.xlsx
+++ b/GoogleOpenImages-allClasses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="839">
   <si>
     <t>class</t>
   </si>
@@ -2379,6 +2379,15 @@
     <t>chest: 4</t>
   </si>
   <si>
+    <t>coffee maker</t>
+  </si>
+  <si>
+    <t>lightbulb</t>
+  </si>
+  <si>
+    <t>salt shaker</t>
+  </si>
+  <si>
     <t>alarm clock</t>
   </si>
   <si>
@@ -2397,9 +2406,6 @@
     <t>faucet</t>
   </si>
   <si>
-    <t>Water tap</t>
-  </si>
-  <si>
     <t>Toilet</t>
   </si>
   <si>
@@ -2451,16 +2457,10 @@
     <t xml:space="preserve">sandal </t>
   </si>
   <si>
-    <t>doughtnut</t>
-  </si>
-  <si>
     <t>microwave oven</t>
   </si>
   <si>
-    <t>lightbulb</t>
-  </si>
-  <si>
-    <t>Cup</t>
+    <t>orange (fruit)</t>
   </si>
   <si>
     <t>swimsuit</t>
@@ -2490,9 +2490,6 @@
     <t>shower curtain</t>
   </si>
   <si>
-    <t>salt shaker</t>
-  </si>
-  <si>
     <t>bath towel</t>
   </si>
   <si>
@@ -2506,9 +2503,6 @@
   </si>
   <si>
     <t>pan</t>
-  </si>
-  <si>
-    <t>coffee maker</t>
   </si>
   <si>
     <t>life jacket</t>
@@ -2826,7 +2820,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3028,6 +3022,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -19849,7 +19846,9 @@
       <c r="D125" s="1">
         <v>20.0</v>
       </c>
-      <c r="E125" s="6"/>
+      <c r="E125" s="72" t="s">
+        <v>785</v>
+      </c>
       <c r="F125" s="9">
         <v>1.0</v>
       </c>
@@ -23225,7 +23224,7 @@
         <v>17.0</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>371</v>
+        <v>786</v>
       </c>
       <c r="F310" s="3">
         <v>1.0</v>
@@ -25432,7 +25431,7 @@
         <v>2.0</v>
       </c>
       <c r="E433" s="14" t="s">
-        <v>500</v>
+        <v>787</v>
       </c>
       <c r="F433" s="8">
         <v>1.0</v>
@@ -28544,11 +28543,11 @@
     </row>
     <row r="603" ht="14.25" customHeight="1"/>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="A604" s="72"/>
+      <c r="A604" s="73"/>
       <c r="D604" s="57"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="A605" s="73"/>
+      <c r="A605" s="74"/>
       <c r="D605" s="65"/>
     </row>
     <row r="606" ht="14.25" customHeight="1">
@@ -28556,23 +28555,23 @@
       <c r="D606" s="66"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="A607" s="72"/>
+      <c r="A607" s="73"/>
       <c r="D607" s="65"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="A608" s="72"/>
+      <c r="A608" s="73"/>
       <c r="D608" s="62"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="A609" s="72"/>
+      <c r="A609" s="73"/>
       <c r="D609" s="57"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="A610" s="72"/>
+      <c r="A610" s="73"/>
       <c r="D610" s="57"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="A611" s="74"/>
+      <c r="A611" s="75"/>
       <c r="D611" s="57"/>
     </row>
     <row r="612" ht="14.25" customHeight="1">
@@ -28580,38 +28579,38 @@
       <c r="D612" s="65"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="A613" s="72"/>
+      <c r="A613" s="73"/>
       <c r="D613" s="62"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="A614" s="75"/>
+      <c r="A614" s="76"/>
       <c r="D614" s="55"/>
     </row>
     <row r="615" ht="14.25" customHeight="1">
       <c r="D615" s="57"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="A616" s="75"/>
+      <c r="A616" s="76"/>
       <c r="D616" s="55"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="A617" s="76"/>
+      <c r="A617" s="77"/>
       <c r="D617" s="65"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="A618" s="72"/>
+      <c r="A618" s="73"/>
       <c r="D618" s="65"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="A619" s="72"/>
+      <c r="A619" s="73"/>
       <c r="D619" s="65"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="A620" s="76"/>
+      <c r="A620" s="77"/>
       <c r="D620" s="65"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="A621" s="72"/>
+      <c r="A621" s="73"/>
       <c r="D621" s="61"/>
     </row>
     <row r="622" ht="14.25" customHeight="1">
@@ -28626,11 +28625,11 @@
       <c r="D624" s="57"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="A625" s="77"/>
+      <c r="A625" s="78"/>
       <c r="D625" s="57"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="A626" s="78"/>
+      <c r="A626" s="79"/>
       <c r="D626" s="61"/>
     </row>
     <row r="627" ht="14.25" customHeight="1">
@@ -28647,16 +28646,16 @@
       <c r="D630" s="70"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="A631" s="74"/>
+      <c r="A631" s="75"/>
       <c r="D631" s="70"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="A632" s="77"/>
-      <c r="D632" s="79"/>
+      <c r="A632" s="78"/>
+      <c r="D632" s="80"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
       <c r="A633" s="69"/>
-      <c r="D633" s="79"/>
+      <c r="D633" s="80"/>
     </row>
     <row r="634" ht="14.25" customHeight="1"/>
     <row r="635" ht="14.25" customHeight="1"/>
@@ -29085,13 +29084,13 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="80" t="s">
-        <v>785</v>
-      </c>
-      <c r="B2" s="80">
+      <c r="A2" s="81" t="s">
+        <v>788</v>
+      </c>
+      <c r="B2" s="81">
         <v>164.0</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="82" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3">
@@ -29102,13 +29101,13 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="80" t="s">
-        <v>786</v>
-      </c>
-      <c r="B3" s="80">
+      <c r="A3" s="81" t="s">
+        <v>789</v>
+      </c>
+      <c r="B3" s="81">
         <v>2246.0</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="82" t="s">
         <v>481</v>
       </c>
       <c r="J3" s="3">
@@ -29116,91 +29115,91 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="81" t="s">
         <v>546</v>
       </c>
-      <c r="B4" s="80">
+      <c r="B4" s="81">
         <v>2231.0</v>
       </c>
-      <c r="C4" s="82"/>
+      <c r="C4" s="83"/>
       <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="81" t="s">
         <v>531</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="81">
         <v>2216.0</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="83"/>
       <c r="J5" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="84" t="s">
         <v>685</v>
       </c>
-      <c r="B6" s="80">
+      <c r="B6" s="81">
         <v>2215.0</v>
       </c>
-      <c r="C6" s="82"/>
+      <c r="C6" s="83"/>
       <c r="J6" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="80">
+      <c r="B7" s="81">
         <v>2214.0</v>
       </c>
-      <c r="C7" s="82"/>
+      <c r="C7" s="83"/>
       <c r="E7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="84"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="82"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="81" t="s">
         <v>455</v>
       </c>
-      <c r="B9" s="80">
+      <c r="B9" s="81">
         <v>2213.0</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="80">
+      <c r="B10" s="81">
         <v>2203.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="83"/>
       <c r="E10" s="19"/>
       <c r="G10" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="81" t="s">
         <v>636</v>
       </c>
-      <c r="B11" s="80">
+      <c r="B11" s="81">
         <v>2203.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="83"/>
       <c r="E11" s="3">
         <v>1.0</v>
       </c>
@@ -29209,25 +29208,25 @@
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="81" t="s">
         <v>653</v>
       </c>
-      <c r="B12" s="80">
+      <c r="B12" s="81">
         <v>2193.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="83"/>
       <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="80">
+      <c r="B13" s="81">
         <v>2182.0</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="3">
         <v>1.0</v>
       </c>
@@ -29239,1843 +29238,1843 @@
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="81" t="s">
+        <v>790</v>
+      </c>
+      <c r="B14" s="81">
+        <v>2190.0</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="84" t="s">
+        <v>791</v>
+      </c>
+      <c r="B15" s="81">
+        <v>2188.0</v>
+      </c>
+      <c r="C15" s="82" t="s">
+        <v>792</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="81" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="81">
+        <v>2182.0</v>
+      </c>
+      <c r="C16" s="83"/>
+      <c r="G16" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="84" t="s">
+        <v>694</v>
+      </c>
+      <c r="B17" s="81">
+        <v>2178.0</v>
+      </c>
+      <c r="C17" s="83"/>
+      <c r="G17" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="81" t="s">
+        <v>525</v>
+      </c>
+      <c r="B18" s="81">
+        <v>2174.0</v>
+      </c>
+      <c r="C18" s="83"/>
+      <c r="G18" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="81" t="s">
+        <v>532</v>
+      </c>
+      <c r="B19" s="81">
+        <v>2171.0</v>
+      </c>
+      <c r="C19" s="83"/>
+      <c r="J19" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="81" t="s">
+        <v>413</v>
+      </c>
+      <c r="B20" s="81">
+        <v>2167.0</v>
+      </c>
+      <c r="C20" s="83"/>
+      <c r="G20" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="81">
+        <v>2163.0</v>
+      </c>
+      <c r="C21" s="83"/>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="81" t="s">
+        <v>459</v>
+      </c>
+      <c r="B22" s="81">
+        <v>2163.0</v>
+      </c>
+      <c r="C22" s="83"/>
+      <c r="H22" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="81" t="s">
+        <v>793</v>
+      </c>
+      <c r="B23" s="81">
+        <v>2162.0</v>
+      </c>
+      <c r="C23" s="82" t="s">
+        <v>593</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="81">
+        <v>2157.0</v>
+      </c>
+      <c r="C24" s="83"/>
+      <c r="D24" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="84" t="s">
+        <v>698</v>
+      </c>
+      <c r="B25" s="81">
+        <v>2155.0</v>
+      </c>
+      <c r="C25" s="83"/>
+      <c r="D25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="81" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" s="81">
+        <v>2152.0</v>
+      </c>
+      <c r="C26" s="83"/>
+      <c r="G26" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="81" t="s">
+        <v>794</v>
+      </c>
+      <c r="B27" s="81">
+        <v>2152.0</v>
+      </c>
+      <c r="C27" s="83"/>
+      <c r="D27" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="81" t="s">
+        <v>639</v>
+      </c>
+      <c r="B28" s="81">
+        <v>2138.0</v>
+      </c>
+      <c r="C28" s="83"/>
+      <c r="D28" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="81">
+        <v>2140.0</v>
+      </c>
+      <c r="C29" s="83"/>
+      <c r="D29" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="81" t="s">
+        <v>795</v>
+      </c>
+      <c r="B30" s="81">
+        <v>2133.0</v>
+      </c>
+      <c r="C30" s="83"/>
+      <c r="G30" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="81" t="s">
+        <v>398</v>
+      </c>
+      <c r="B31" s="81">
+        <v>2132.0</v>
+      </c>
+      <c r="C31" s="83"/>
+      <c r="D31" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="84" t="s">
+        <v>796</v>
+      </c>
+      <c r="B32" s="81">
+        <v>2129.0</v>
+      </c>
+      <c r="C32" s="83"/>
+      <c r="E32" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="81" t="s">
+        <v>577</v>
+      </c>
+      <c r="B33" s="81">
+        <v>2127.0</v>
+      </c>
+      <c r="C33" s="83"/>
+      <c r="J33" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="81" t="s">
+        <v>355</v>
+      </c>
+      <c r="B34" s="81">
+        <v>2125.0</v>
+      </c>
+      <c r="C34" s="83"/>
+      <c r="D34" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="81">
+        <v>2115.0</v>
+      </c>
+      <c r="C35" s="83"/>
+      <c r="I35" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="81" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="81">
+        <v>2114.0</v>
+      </c>
+      <c r="C36" s="83"/>
+      <c r="D36" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="B37" s="81">
+        <v>2113.0</v>
+      </c>
+      <c r="C37" s="83"/>
+      <c r="I37" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="81">
+        <v>2106.0</v>
+      </c>
+      <c r="C38" s="83"/>
+      <c r="D38" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="84" t="s">
+        <v>703</v>
+      </c>
+      <c r="B39" s="81">
+        <v>2088.0</v>
+      </c>
+      <c r="C39" s="83"/>
+      <c r="G39" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="81" t="s">
+        <v>363</v>
+      </c>
+      <c r="B40" s="81">
+        <v>2067.0</v>
+      </c>
+      <c r="C40" s="83"/>
+      <c r="D40" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="A41" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="81">
+        <v>1997.0</v>
+      </c>
+      <c r="C41" s="83"/>
+      <c r="H41" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="81">
+        <v>1997.0</v>
+      </c>
+      <c r="C42" s="83"/>
+      <c r="D42" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="81" t="s">
+        <v>797</v>
+      </c>
+      <c r="B43" s="81">
+        <v>1995.0</v>
+      </c>
+      <c r="C43" s="83"/>
+      <c r="J43" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="84" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="81">
+        <v>1948.0</v>
+      </c>
+      <c r="C44" s="83"/>
+      <c r="D44" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="81" t="s">
+        <v>798</v>
+      </c>
+      <c r="B45" s="81">
+        <v>1920.0</v>
+      </c>
+      <c r="C45" s="83"/>
+      <c r="D45" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="81" t="s">
+        <v>675</v>
+      </c>
+      <c r="B46" s="81">
+        <v>1902.0</v>
+      </c>
+      <c r="C46" s="83"/>
+      <c r="I46" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="84" t="s">
+        <v>710</v>
+      </c>
+      <c r="B47" s="81">
+        <v>1877.0</v>
+      </c>
+      <c r="C47" s="83"/>
+      <c r="G47" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="81" t="s">
+        <v>530</v>
+      </c>
+      <c r="B48" s="81">
+        <v>1869.0</v>
+      </c>
+      <c r="C48" s="83"/>
+      <c r="D48" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="81" t="s">
+        <v>574</v>
+      </c>
+      <c r="B49" s="81">
+        <v>1831.0</v>
+      </c>
+      <c r="C49" s="83"/>
+      <c r="D49" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="84" t="s">
+        <v>799</v>
+      </c>
+      <c r="B50" s="81">
+        <v>1784.0</v>
+      </c>
+      <c r="C50" s="83"/>
+      <c r="G50" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="81">
+        <v>1709.0</v>
+      </c>
+      <c r="C51" s="83"/>
+      <c r="H51" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="81">
+        <v>1698.0</v>
+      </c>
+      <c r="C52" s="83"/>
+      <c r="D52" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="81">
+        <v>1664.0</v>
+      </c>
+      <c r="C53" s="83"/>
+      <c r="G53" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="81" t="s">
+        <v>487</v>
+      </c>
+      <c r="B54" s="81">
+        <v>1655.0</v>
+      </c>
+      <c r="C54" s="83"/>
+      <c r="D54" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="81" t="s">
+        <v>800</v>
+      </c>
+      <c r="B55" s="81">
+        <v>1640.0</v>
+      </c>
+      <c r="C55" s="83"/>
+      <c r="D55" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="56" ht="14.25" customHeight="1">
+      <c r="A56" s="84" t="s">
+        <v>801</v>
+      </c>
+      <c r="B56" s="81">
+        <v>1639.0</v>
+      </c>
+      <c r="C56" s="83"/>
+      <c r="G56" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="A57" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="81">
+        <v>1611.0</v>
+      </c>
+      <c r="C57" s="83"/>
+      <c r="I57" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="A58" s="81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="81">
+        <v>1578.0</v>
+      </c>
+      <c r="C58" s="83"/>
+      <c r="G58" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="A59" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="81">
+        <v>1520.0</v>
+      </c>
+      <c r="C59" s="83"/>
+      <c r="H59" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" s="81" t="s">
+        <v>802</v>
+      </c>
+      <c r="B60" s="81">
+        <v>1482.0</v>
+      </c>
+      <c r="C60" s="83"/>
+      <c r="J60" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="81" t="s">
+        <v>803</v>
+      </c>
+      <c r="B61" s="81">
+        <v>1383.0</v>
+      </c>
+      <c r="C61" s="83"/>
+      <c r="H61" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="81">
+        <v>1382.0</v>
+      </c>
+      <c r="C62" s="83"/>
+      <c r="H62" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="81">
+        <v>1339.0</v>
+      </c>
+      <c r="C63" s="83"/>
+      <c r="H63" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="81" t="s">
+        <v>553</v>
+      </c>
+      <c r="B64" s="81">
+        <v>1287.0</v>
+      </c>
+      <c r="C64" s="83"/>
+      <c r="D64" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="81" t="s">
+        <v>804</v>
+      </c>
+      <c r="B65" s="81">
+        <v>1273.0</v>
+      </c>
+      <c r="C65" s="83"/>
+      <c r="D65" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="81">
+        <v>1257.0</v>
+      </c>
+      <c r="C66" s="83"/>
+      <c r="D66" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="84" t="s">
+        <v>723</v>
+      </c>
+      <c r="B67" s="81">
+        <v>1247.0</v>
+      </c>
+      <c r="C67" s="83"/>
+      <c r="E67" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" s="86" t="s">
+        <v>805</v>
+      </c>
+      <c r="B68" s="81">
+        <v>1227.0</v>
+      </c>
+      <c r="C68" s="83"/>
+      <c r="G68" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="B69" s="81">
+        <v>1170.0</v>
+      </c>
+      <c r="C69" s="83"/>
+      <c r="D69" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" s="81" t="s">
+        <v>806</v>
+      </c>
+      <c r="B70" s="81">
+        <v>1164.0</v>
+      </c>
+      <c r="C70" s="82" t="s">
+        <v>807</v>
+      </c>
+      <c r="D70" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="84" t="s">
+        <v>728</v>
+      </c>
+      <c r="B71" s="81">
+        <v>1130.0</v>
+      </c>
+      <c r="C71" s="82" t="s">
+        <v>808</v>
+      </c>
+      <c r="D71" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="81" t="s">
+        <v>809</v>
+      </c>
+      <c r="B72" s="81">
+        <v>1129.0</v>
+      </c>
+      <c r="C72" s="83"/>
+      <c r="E72" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J72" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="81" t="s">
+        <v>810</v>
+      </c>
+      <c r="B73" s="81">
+        <v>1124.0</v>
+      </c>
+      <c r="C73" s="83"/>
+      <c r="G73" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="81">
+        <v>1102.0</v>
+      </c>
+      <c r="C74" s="83"/>
+      <c r="H74" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="75" ht="14.25" customHeight="1">
+      <c r="A75" s="81" t="s">
+        <v>811</v>
+      </c>
+      <c r="B75" s="81">
+        <v>1097.0</v>
+      </c>
+      <c r="C75" s="83"/>
+      <c r="D75" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="84" t="s">
+        <v>729</v>
+      </c>
+      <c r="B76" s="81">
+        <v>1089.0</v>
+      </c>
+      <c r="C76" s="83"/>
+      <c r="G76" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" s="81" t="s">
+        <v>522</v>
+      </c>
+      <c r="B77" s="81">
+        <v>1075.0</v>
+      </c>
+      <c r="C77" s="83"/>
+      <c r="I77" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" s="81" t="s">
+        <v>519</v>
+      </c>
+      <c r="B78" s="81">
+        <v>1033.0</v>
+      </c>
+      <c r="C78" s="83"/>
+      <c r="D78" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" s="81" t="s">
+        <v>786</v>
+      </c>
+      <c r="B79" s="81">
+        <v>991.0</v>
+      </c>
+      <c r="C79" s="83"/>
+      <c r="D79" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="A80" s="84" t="s">
+        <v>730</v>
+      </c>
+      <c r="B80" s="81">
+        <v>978.0</v>
+      </c>
+      <c r="C80" s="83"/>
+      <c r="G80" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="A81" s="81" t="s">
+        <v>407</v>
+      </c>
+      <c r="B81" s="81">
+        <v>933.0</v>
+      </c>
+      <c r="C81" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25" customHeight="1">
+      <c r="A82" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" s="81">
+        <v>929.0</v>
+      </c>
+      <c r="C82" s="83"/>
+      <c r="D82" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25" customHeight="1">
+      <c r="A83" s="81" t="s">
+        <v>812</v>
+      </c>
+      <c r="B83" s="81">
+        <v>921.0</v>
+      </c>
+      <c r="C83" s="83"/>
+      <c r="H83" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" s="81" t="s">
+        <v>102</v>
+      </c>
+      <c r="B84" s="81">
+        <v>918.0</v>
+      </c>
+      <c r="C84" s="83"/>
+      <c r="H84" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" s="81" t="s">
+        <v>813</v>
+      </c>
+      <c r="B85" s="81">
+        <v>892.0</v>
+      </c>
+      <c r="C85" s="83"/>
+      <c r="G85" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="A86" s="87" t="s">
+        <v>506</v>
+      </c>
+      <c r="B86" s="81">
+        <v>863.0</v>
+      </c>
+      <c r="C86" s="83"/>
+      <c r="G86" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="A87" s="81" t="s">
+        <v>144</v>
+      </c>
+      <c r="B87" s="81">
+        <v>831.0</v>
+      </c>
+      <c r="C87" s="83"/>
+      <c r="G87" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="A88" s="81" t="s">
+        <v>616</v>
+      </c>
+      <c r="B88" s="81">
+        <v>831.0</v>
+      </c>
+      <c r="C88" s="83"/>
+      <c r="D88" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25" customHeight="1">
+      <c r="A89" s="81" t="s">
+        <v>507</v>
+      </c>
+      <c r="B89" s="81">
+        <v>804.0</v>
+      </c>
+      <c r="C89" s="83"/>
+      <c r="D89" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25" customHeight="1">
+      <c r="A90" s="84" t="s">
+        <v>731</v>
+      </c>
+      <c r="B90" s="81">
+        <v>801.0</v>
+      </c>
+      <c r="C90" s="83"/>
+      <c r="D90" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E90" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="91" ht="14.25" customHeight="1">
+      <c r="A91" s="81" t="s">
+        <v>423</v>
+      </c>
+      <c r="B91" s="81">
+        <v>776.0</v>
+      </c>
+      <c r="C91" s="83"/>
+      <c r="D91" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="92" ht="14.25" customHeight="1">
+      <c r="A92" s="84" t="s">
+        <v>814</v>
+      </c>
+      <c r="B92" s="81">
+        <v>772.0</v>
+      </c>
+      <c r="C92" s="83"/>
+      <c r="G92" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="93" ht="14.25" customHeight="1">
+      <c r="A93" s="81" t="s">
+        <v>815</v>
+      </c>
+      <c r="B93" s="81">
+        <v>770.0</v>
+      </c>
+      <c r="C93" s="82" t="s">
+        <v>498</v>
+      </c>
+      <c r="H93" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="94" ht="14.25" customHeight="1">
+      <c r="A94" s="81" t="s">
+        <v>816</v>
+      </c>
+      <c r="B94" s="81">
+        <v>739.0</v>
+      </c>
+      <c r="C94" s="83"/>
+      <c r="H94" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="95" ht="14.25" customHeight="1">
+      <c r="A95" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95" s="81">
+        <v>735.0</v>
+      </c>
+      <c r="C95" s="83"/>
+      <c r="I95" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="96" ht="14.25" customHeight="1">
+      <c r="A96" s="81" t="s">
+        <v>817</v>
+      </c>
+      <c r="B96" s="81">
+        <v>732.0</v>
+      </c>
+      <c r="C96" s="83"/>
+      <c r="D96" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="97" ht="14.25" customHeight="1">
+      <c r="A97" s="84" t="s">
+        <v>734</v>
+      </c>
+      <c r="B97" s="81">
+        <v>727.0</v>
+      </c>
+      <c r="C97" s="83"/>
+      <c r="E97" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="98" ht="14.25" customHeight="1">
+      <c r="A98" s="81" t="s">
+        <v>619</v>
+      </c>
+      <c r="B98" s="81">
+        <v>719.0</v>
+      </c>
+      <c r="C98" s="83"/>
+      <c r="D98" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I98" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25" customHeight="1">
+      <c r="A99" s="81" t="s">
+        <v>360</v>
+      </c>
+      <c r="B99" s="81">
+        <v>710.0</v>
+      </c>
+      <c r="C99" s="83"/>
+      <c r="D99" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E99" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25" customHeight="1">
+      <c r="A100" s="84" t="s">
+        <v>736</v>
+      </c>
+      <c r="B100" s="81">
+        <v>696.0</v>
+      </c>
+      <c r="C100" s="83"/>
+      <c r="H100" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="101" ht="14.25" customHeight="1">
+      <c r="A101" s="84" t="s">
+        <v>738</v>
+      </c>
+      <c r="B101" s="81">
+        <v>695.0</v>
+      </c>
+      <c r="C101" s="83"/>
+      <c r="E101" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="102" ht="14.25" customHeight="1">
+      <c r="A102" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="B102" s="81">
+        <v>674.0</v>
+      </c>
+      <c r="C102" s="83"/>
+      <c r="D102" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="A103" s="84" t="s">
+        <v>740</v>
+      </c>
+      <c r="B103" s="81">
+        <v>653.0</v>
+      </c>
+      <c r="C103" s="83"/>
+      <c r="G103" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="A104" s="81" t="s">
+        <v>228</v>
+      </c>
+      <c r="B104" s="81">
+        <v>603.0</v>
+      </c>
+      <c r="C104" s="83"/>
+      <c r="D104" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="105" ht="14.25" customHeight="1">
+      <c r="A105" s="84" t="s">
+        <v>742</v>
+      </c>
+      <c r="B105" s="81">
+        <v>598.0</v>
+      </c>
+      <c r="C105" s="83"/>
+      <c r="D105" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="106" ht="14.25" customHeight="1">
+      <c r="A106" s="84" t="s">
+        <v>744</v>
+      </c>
+      <c r="B106" s="81">
+        <v>588.0</v>
+      </c>
+      <c r="C106" s="83"/>
+      <c r="J106" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25" customHeight="1">
+      <c r="A107" s="86" t="s">
+        <v>746</v>
+      </c>
+      <c r="B107" s="81">
+        <v>588.0</v>
+      </c>
+      <c r="C107" s="83"/>
+      <c r="E107" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="A108" s="84" t="s">
+        <v>748</v>
+      </c>
+      <c r="B108" s="81">
+        <v>565.0</v>
+      </c>
+      <c r="C108" s="83"/>
+      <c r="G108" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J108" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="109" ht="14.25" customHeight="1">
+      <c r="A109" s="84" t="s">
+        <v>750</v>
+      </c>
+      <c r="B109" s="81">
+        <v>561.0</v>
+      </c>
+      <c r="C109" s="83"/>
+      <c r="D109" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G109" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="A110" s="81" t="s">
+        <v>818</v>
+      </c>
+      <c r="B110" s="81">
+        <v>546.0</v>
+      </c>
+      <c r="C110" s="83"/>
+      <c r="D110" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="111" ht="14.25" customHeight="1">
+      <c r="A111" s="81" t="s">
+        <v>819</v>
+      </c>
+      <c r="B111" s="81">
+        <v>502.0</v>
+      </c>
+      <c r="C111" s="82" t="s">
+        <v>609</v>
+      </c>
+      <c r="D111" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="112" ht="14.25" customHeight="1">
+      <c r="A112" s="84" t="s">
+        <v>753</v>
+      </c>
+      <c r="B112" s="81">
+        <v>480.0</v>
+      </c>
+      <c r="C112" s="83"/>
+      <c r="D112" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E112" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="113" ht="14.25" customHeight="1">
+      <c r="A113" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="B113" s="81">
+        <v>473.0</v>
+      </c>
+      <c r="C113" s="83"/>
+    </row>
+    <row r="114" ht="14.25" customHeight="1">
+      <c r="A114" s="81" t="s">
+        <v>820</v>
+      </c>
+      <c r="B114" s="81">
+        <v>432.0</v>
+      </c>
+      <c r="C114" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="D114" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="115" ht="14.25" customHeight="1">
+      <c r="A115" s="81" t="s">
+        <v>821</v>
+      </c>
+      <c r="B115" s="81">
+        <v>424.0</v>
+      </c>
+      <c r="C115" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="D115" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="116" ht="14.25" customHeight="1">
+      <c r="A116" s="81" t="s">
         <v>787</v>
       </c>
-      <c r="B14" s="80">
-        <v>2190.0</v>
-      </c>
-      <c r="C14" s="81" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="83" t="s">
-        <v>788</v>
-      </c>
-      <c r="B15" s="80">
-        <v>2188.0</v>
-      </c>
-      <c r="C15" s="81" t="s">
-        <v>789</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="B16" s="80">
-        <v>2182.0</v>
-      </c>
-      <c r="C16" s="82"/>
-      <c r="G16" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="83" t="s">
-        <v>694</v>
-      </c>
-      <c r="B17" s="80">
-        <v>2178.0</v>
-      </c>
-      <c r="C17" s="82"/>
-      <c r="G17" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="80" t="s">
-        <v>525</v>
-      </c>
-      <c r="B18" s="80">
-        <v>2174.0</v>
-      </c>
-      <c r="C18" s="82"/>
-      <c r="G18" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="80" t="s">
-        <v>532</v>
-      </c>
-      <c r="B19" s="80">
-        <v>2171.0</v>
-      </c>
-      <c r="C19" s="82"/>
-      <c r="J19" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="80" t="s">
-        <v>413</v>
-      </c>
-      <c r="B20" s="80">
-        <v>2167.0</v>
-      </c>
-      <c r="C20" s="82"/>
-      <c r="G20" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="80">
-        <v>2163.0</v>
-      </c>
-      <c r="C21" s="82"/>
-      <c r="D21" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="80" t="s">
-        <v>459</v>
-      </c>
-      <c r="B22" s="80">
-        <v>2163.0</v>
-      </c>
-      <c r="C22" s="82"/>
-      <c r="H22" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="80" t="s">
-        <v>790</v>
-      </c>
-      <c r="B23" s="80">
-        <v>2162.0</v>
-      </c>
-      <c r="C23" s="81" t="s">
-        <v>791</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="80" t="s">
-        <v>205</v>
-      </c>
-      <c r="B24" s="80">
-        <v>2157.0</v>
-      </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="83" t="s">
-        <v>698</v>
-      </c>
-      <c r="B25" s="80">
-        <v>2155.0</v>
-      </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="B26" s="80">
-        <v>2152.0</v>
-      </c>
-      <c r="C26" s="82"/>
-      <c r="G26" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="80" t="s">
-        <v>792</v>
-      </c>
-      <c r="B27" s="80">
-        <v>2152.0</v>
-      </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="80" t="s">
-        <v>639</v>
-      </c>
-      <c r="B28" s="80">
-        <v>2138.0</v>
-      </c>
-      <c r="C28" s="82"/>
-      <c r="D28" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="80" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" s="80">
-        <v>2140.0</v>
-      </c>
-      <c r="C29" s="82"/>
-      <c r="D29" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="80" t="s">
-        <v>793</v>
-      </c>
-      <c r="B30" s="80">
-        <v>2133.0</v>
-      </c>
-      <c r="C30" s="82"/>
-      <c r="G30" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="80" t="s">
-        <v>398</v>
-      </c>
-      <c r="B31" s="80">
-        <v>2132.0</v>
-      </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="83" t="s">
-        <v>794</v>
-      </c>
-      <c r="B32" s="80">
-        <v>2129.0</v>
-      </c>
-      <c r="C32" s="82"/>
-      <c r="E32" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="80" t="s">
-        <v>577</v>
-      </c>
-      <c r="B33" s="80">
-        <v>2127.0</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="J33" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="80" t="s">
-        <v>355</v>
-      </c>
-      <c r="B34" s="80">
-        <v>2125.0</v>
-      </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="80" t="s">
-        <v>215</v>
-      </c>
-      <c r="B35" s="80">
-        <v>2115.0</v>
-      </c>
-      <c r="C35" s="82"/>
-      <c r="I35" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="80" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="80">
-        <v>2114.0</v>
-      </c>
-      <c r="C36" s="82"/>
-      <c r="D36" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="B37" s="80">
-        <v>2113.0</v>
-      </c>
-      <c r="C37" s="82"/>
-      <c r="I37" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="80">
-        <v>2106.0</v>
-      </c>
-      <c r="C38" s="82"/>
-      <c r="D38" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="83" t="s">
-        <v>703</v>
-      </c>
-      <c r="B39" s="80">
-        <v>2088.0</v>
-      </c>
-      <c r="C39" s="82"/>
-      <c r="G39" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="80" t="s">
-        <v>363</v>
-      </c>
-      <c r="B40" s="80">
-        <v>2067.0</v>
-      </c>
-      <c r="C40" s="82"/>
-      <c r="D40" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="80">
-        <v>1997.0</v>
-      </c>
-      <c r="C41" s="82"/>
-      <c r="H41" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="80" t="s">
+      <c r="B116" s="81">
+        <v>418.0</v>
+      </c>
+      <c r="C116" s="83"/>
+      <c r="D116" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="117" ht="14.25" customHeight="1">
+      <c r="A117" s="84" t="s">
+        <v>822</v>
+      </c>
+      <c r="B117" s="81">
+        <v>405.0</v>
+      </c>
+      <c r="C117" s="82" t="s">
+        <v>619</v>
+      </c>
+      <c r="D117" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J117" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="118" ht="14.25" customHeight="1">
+      <c r="A118" s="81" t="s">
+        <v>368</v>
+      </c>
+      <c r="B118" s="81">
+        <v>393.0</v>
+      </c>
+      <c r="C118" s="83"/>
+      <c r="H118" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="119" ht="14.25" customHeight="1">
+      <c r="A119" s="81" t="s">
+        <v>440</v>
+      </c>
+      <c r="B119" s="81">
+        <v>382.0</v>
+      </c>
+      <c r="C119" s="83"/>
+      <c r="D119" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="120" ht="14.25" customHeight="1">
+      <c r="A120" s="81" t="s">
+        <v>567</v>
+      </c>
+      <c r="B120" s="81">
+        <v>379.0</v>
+      </c>
+      <c r="C120" s="83"/>
+      <c r="H120" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="121" ht="14.25" customHeight="1">
+      <c r="A121" s="81" t="s">
+        <v>823</v>
+      </c>
+      <c r="B121" s="81">
+        <v>359.0</v>
+      </c>
+      <c r="C121" s="83"/>
+      <c r="H121" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="122" ht="14.25" customHeight="1">
+      <c r="A122" s="81" t="s">
+        <v>550</v>
+      </c>
+      <c r="B122" s="81">
+        <v>353.0</v>
+      </c>
+      <c r="C122" s="83"/>
+      <c r="D122" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="123" ht="14.25" customHeight="1">
+      <c r="A123" s="81" t="s">
+        <v>472</v>
+      </c>
+      <c r="B123" s="81">
+        <v>348.0</v>
+      </c>
+      <c r="C123" s="83"/>
+      <c r="H123" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="124" ht="14.25" customHeight="1">
+      <c r="A124" s="81" t="s">
+        <v>565</v>
+      </c>
+      <c r="B124" s="81">
+        <v>344.0</v>
+      </c>
+      <c r="C124" s="83"/>
+      <c r="D124" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="125" ht="14.25" customHeight="1">
+      <c r="A125" s="81" t="s">
+        <v>394</v>
+      </c>
+      <c r="B125" s="81">
+        <v>315.0</v>
+      </c>
+      <c r="C125" s="83"/>
+      <c r="D125" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="126" ht="14.25" customHeight="1">
+      <c r="A126" s="81" t="s">
+        <v>824</v>
+      </c>
+      <c r="B126" s="81">
+        <v>309.0</v>
+      </c>
+      <c r="C126" s="82" t="s">
+        <v>458</v>
+      </c>
+      <c r="D126" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="127" ht="14.25" customHeight="1">
+      <c r="A127" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="B127" s="81">
+        <v>283.0</v>
+      </c>
+      <c r="C127" s="83"/>
+      <c r="D127" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="128" ht="14.25" customHeight="1">
+      <c r="A128" s="81" t="s">
+        <v>825</v>
+      </c>
+      <c r="B128" s="81">
+        <v>279.0</v>
+      </c>
+      <c r="C128" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="80">
-        <v>1997.0</v>
-      </c>
-      <c r="C42" s="82"/>
-      <c r="D42" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E42" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="80" t="s">
-        <v>795</v>
-      </c>
-      <c r="B43" s="80">
-        <v>1995.0</v>
-      </c>
-      <c r="C43" s="82"/>
-      <c r="J43" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="83" t="s">
-        <v>202</v>
-      </c>
-      <c r="B44" s="80">
-        <v>1948.0</v>
-      </c>
-      <c r="C44" s="82"/>
-      <c r="D44" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E44" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="80" t="s">
-        <v>796</v>
-      </c>
-      <c r="B45" s="80">
-        <v>1920.0</v>
-      </c>
-      <c r="C45" s="82"/>
-      <c r="D45" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="80" t="s">
-        <v>675</v>
-      </c>
-      <c r="B46" s="80">
-        <v>1902.0</v>
-      </c>
-      <c r="C46" s="82"/>
-      <c r="I46" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="83" t="s">
-        <v>710</v>
-      </c>
-      <c r="B47" s="80">
-        <v>1877.0</v>
-      </c>
-      <c r="C47" s="82"/>
-      <c r="G47" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="80" t="s">
-        <v>530</v>
-      </c>
-      <c r="B48" s="80">
-        <v>1869.0</v>
-      </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="80" t="s">
-        <v>574</v>
-      </c>
-      <c r="B49" s="80">
-        <v>1831.0</v>
-      </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="83" t="s">
-        <v>797</v>
-      </c>
-      <c r="B50" s="80">
-        <v>1784.0</v>
-      </c>
-      <c r="C50" s="82"/>
-      <c r="G50" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="80">
-        <v>1709.0</v>
-      </c>
-      <c r="C51" s="82"/>
-      <c r="H51" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" s="80">
-        <v>1698.0</v>
-      </c>
-      <c r="C52" s="82"/>
-      <c r="D52" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="80" t="s">
-        <v>206</v>
-      </c>
-      <c r="B53" s="80">
-        <v>1664.0</v>
-      </c>
-      <c r="C53" s="82"/>
-      <c r="G53" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="80" t="s">
-        <v>487</v>
-      </c>
-      <c r="B54" s="80">
-        <v>1655.0</v>
-      </c>
-      <c r="C54" s="82"/>
-      <c r="D54" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="80" t="s">
-        <v>798</v>
-      </c>
-      <c r="B55" s="80">
-        <v>1640.0</v>
-      </c>
-      <c r="C55" s="82"/>
-      <c r="D55" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="83" t="s">
-        <v>799</v>
-      </c>
-      <c r="B56" s="80">
-        <v>1639.0</v>
-      </c>
-      <c r="C56" s="82"/>
-      <c r="G56" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J56" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="80" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" s="80">
-        <v>1611.0</v>
-      </c>
-      <c r="C57" s="82"/>
-      <c r="I57" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="80" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="80">
-        <v>1578.0</v>
-      </c>
-      <c r="C58" s="82"/>
-      <c r="G58" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="80">
-        <v>1520.0</v>
-      </c>
-      <c r="C59" s="82"/>
-      <c r="H59" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="80" t="s">
-        <v>800</v>
-      </c>
-      <c r="B60" s="80">
-        <v>1482.0</v>
-      </c>
-      <c r="C60" s="82"/>
-      <c r="J60" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="80" t="s">
-        <v>801</v>
-      </c>
-      <c r="B61" s="80">
-        <v>1383.0</v>
-      </c>
-      <c r="C61" s="82"/>
-      <c r="H61" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" s="80">
-        <v>1382.0</v>
-      </c>
-      <c r="C62" s="82"/>
-      <c r="H62" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" s="80">
-        <v>1339.0</v>
-      </c>
-      <c r="C63" s="82"/>
-      <c r="H63" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="80" t="s">
-        <v>553</v>
-      </c>
-      <c r="B64" s="80">
-        <v>1287.0</v>
-      </c>
-      <c r="C64" s="82"/>
-      <c r="D64" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="80" t="s">
-        <v>802</v>
-      </c>
-      <c r="B65" s="80">
-        <v>1273.0</v>
-      </c>
-      <c r="C65" s="82"/>
-      <c r="D65" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="B66" s="80">
-        <v>1257.0</v>
-      </c>
-      <c r="C66" s="82"/>
-      <c r="D66" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="83" t="s">
-        <v>723</v>
-      </c>
-      <c r="B67" s="80">
-        <v>1247.0</v>
-      </c>
-      <c r="C67" s="82"/>
-      <c r="E67" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="85" t="s">
-        <v>803</v>
-      </c>
-      <c r="B68" s="80">
-        <v>1227.0</v>
-      </c>
-      <c r="C68" s="82"/>
-      <c r="G68" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="B69" s="80">
-        <v>1170.0</v>
-      </c>
-      <c r="C69" s="82"/>
-      <c r="D69" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="80" t="s">
-        <v>804</v>
-      </c>
-      <c r="B70" s="80">
-        <v>1164.0</v>
-      </c>
-      <c r="C70" s="81" t="s">
-        <v>805</v>
-      </c>
-      <c r="D70" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="83" t="s">
-        <v>728</v>
-      </c>
-      <c r="B71" s="80">
-        <v>1130.0</v>
-      </c>
-      <c r="C71" s="81" t="s">
-        <v>806</v>
-      </c>
-      <c r="D71" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="80" t="s">
-        <v>807</v>
-      </c>
-      <c r="B72" s="80">
-        <v>1129.0</v>
-      </c>
-      <c r="C72" s="82"/>
-      <c r="E72" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J72" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="80" t="s">
-        <v>808</v>
-      </c>
-      <c r="B73" s="80">
-        <v>1124.0</v>
-      </c>
-      <c r="C73" s="82"/>
-      <c r="G73" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="80" t="s">
-        <v>809</v>
-      </c>
-      <c r="B74" s="80">
-        <v>1102.0</v>
-      </c>
-      <c r="C74" s="82"/>
-      <c r="H74" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="80" t="s">
-        <v>810</v>
-      </c>
-      <c r="B75" s="80">
-        <v>1097.0</v>
-      </c>
-      <c r="C75" s="82"/>
-      <c r="D75" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="83" t="s">
-        <v>729</v>
-      </c>
-      <c r="B76" s="80">
-        <v>1089.0</v>
-      </c>
-      <c r="C76" s="82"/>
-      <c r="G76" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="80" t="s">
-        <v>522</v>
-      </c>
-      <c r="B77" s="80">
-        <v>1075.0</v>
-      </c>
-      <c r="C77" s="82"/>
-      <c r="I77" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="80" t="s">
-        <v>519</v>
-      </c>
-      <c r="B78" s="80">
-        <v>1033.0</v>
-      </c>
-      <c r="C78" s="82"/>
-      <c r="D78" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="80" t="s">
-        <v>811</v>
-      </c>
-      <c r="B79" s="80">
-        <v>991.0</v>
-      </c>
-      <c r="C79" s="82"/>
-      <c r="D79" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="83" t="s">
-        <v>730</v>
-      </c>
-      <c r="B80" s="80">
-        <v>978.0</v>
-      </c>
-      <c r="C80" s="82"/>
-      <c r="G80" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="80" t="s">
-        <v>407</v>
-      </c>
-      <c r="B81" s="80">
-        <v>933.0</v>
-      </c>
-      <c r="C81" s="81" t="s">
-        <v>812</v>
-      </c>
-      <c r="D81" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="B82" s="80">
-        <v>929.0</v>
-      </c>
-      <c r="C82" s="82"/>
-      <c r="D82" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="80" t="s">
-        <v>418</v>
-      </c>
-      <c r="B83" s="80">
-        <v>921.0</v>
-      </c>
-      <c r="C83" s="82"/>
-      <c r="H83" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="B84" s="80">
-        <v>918.0</v>
-      </c>
-      <c r="C84" s="82"/>
-      <c r="H84" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="80" t="s">
-        <v>813</v>
-      </c>
-      <c r="B85" s="80">
-        <v>892.0</v>
-      </c>
-      <c r="C85" s="82"/>
-      <c r="G85" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="86" t="s">
-        <v>506</v>
-      </c>
-      <c r="B86" s="80">
-        <v>863.0</v>
-      </c>
-      <c r="C86" s="82"/>
-      <c r="G86" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="80" t="s">
-        <v>144</v>
-      </c>
-      <c r="B87" s="80">
-        <v>831.0</v>
-      </c>
-      <c r="C87" s="82"/>
-      <c r="G87" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="80" t="s">
-        <v>616</v>
-      </c>
-      <c r="B88" s="80">
-        <v>831.0</v>
-      </c>
-      <c r="C88" s="82"/>
-      <c r="D88" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="80" t="s">
-        <v>507</v>
-      </c>
-      <c r="B89" s="80">
-        <v>804.0</v>
-      </c>
-      <c r="C89" s="82"/>
-      <c r="D89" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="83" t="s">
-        <v>731</v>
-      </c>
-      <c r="B90" s="80">
-        <v>801.0</v>
-      </c>
-      <c r="C90" s="82"/>
-      <c r="D90" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E90" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="80" t="s">
-        <v>423</v>
-      </c>
-      <c r="B91" s="80">
-        <v>776.0</v>
-      </c>
-      <c r="C91" s="82"/>
-      <c r="D91" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="83" t="s">
-        <v>814</v>
-      </c>
-      <c r="B92" s="80">
-        <v>772.0</v>
-      </c>
-      <c r="C92" s="82"/>
-      <c r="G92" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="80" t="s">
-        <v>815</v>
-      </c>
-      <c r="B93" s="80">
-        <v>770.0</v>
-      </c>
-      <c r="C93" s="81" t="s">
-        <v>498</v>
-      </c>
-      <c r="H93" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="80" t="s">
-        <v>816</v>
-      </c>
-      <c r="B94" s="80">
-        <v>739.0</v>
-      </c>
-      <c r="C94" s="82"/>
-      <c r="H94" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="B95" s="80">
-        <v>735.0</v>
-      </c>
-      <c r="C95" s="82"/>
-      <c r="I95" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="80" t="s">
-        <v>817</v>
-      </c>
-      <c r="B96" s="80">
-        <v>732.0</v>
-      </c>
-      <c r="C96" s="82"/>
-      <c r="D96" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="83" t="s">
-        <v>734</v>
-      </c>
-      <c r="B97" s="80">
-        <v>727.0</v>
-      </c>
-      <c r="C97" s="82"/>
-      <c r="E97" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="80" t="s">
+      <c r="D128" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E128" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="129" ht="14.25" customHeight="1">
+      <c r="A129" s="81" t="s">
+        <v>503</v>
+      </c>
+      <c r="B129" s="81">
+        <v>278.0</v>
+      </c>
+      <c r="C129" s="83"/>
+      <c r="D129" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E129" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="130" ht="14.25" customHeight="1">
+      <c r="A130" s="81" t="s">
+        <v>826</v>
+      </c>
+      <c r="B130" s="81">
+        <v>276.0</v>
+      </c>
+      <c r="C130" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="D130" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E130" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="131" ht="14.25" customHeight="1">
+      <c r="A131" s="81" t="s">
+        <v>182</v>
+      </c>
+      <c r="B131" s="81">
+        <v>274.0</v>
+      </c>
+      <c r="C131" s="83"/>
+      <c r="H131" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25" customHeight="1">
+      <c r="A132" s="81" t="s">
+        <v>785</v>
+      </c>
+      <c r="B132" s="81">
+        <v>264.0</v>
+      </c>
+      <c r="C132" s="83"/>
+      <c r="D132" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25" customHeight="1">
+      <c r="A133" s="81" t="s">
+        <v>270</v>
+      </c>
+      <c r="B133" s="81">
+        <v>262.0</v>
+      </c>
+      <c r="C133" s="83"/>
+      <c r="H133" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="134" ht="14.25" customHeight="1">
+      <c r="A134" s="81" t="s">
+        <v>827</v>
+      </c>
+      <c r="B134" s="81">
+        <v>250.0</v>
+      </c>
+      <c r="C134" s="83"/>
+      <c r="G134" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="135" ht="14.25" customHeight="1">
+      <c r="A135" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="B135" s="81">
+        <v>247.0</v>
+      </c>
+      <c r="C135" s="83"/>
+      <c r="E135" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="136" ht="14.25" customHeight="1">
+      <c r="A136" s="81" t="s">
+        <v>828</v>
+      </c>
+      <c r="B136" s="81">
+        <v>229.0</v>
+      </c>
+      <c r="C136" s="82" t="s">
         <v>619</v>
       </c>
-      <c r="B98" s="80">
-        <v>719.0</v>
-      </c>
-      <c r="C98" s="82"/>
-      <c r="D98" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I98" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="80" t="s">
-        <v>360</v>
-      </c>
-      <c r="B99" s="80">
-        <v>710.0</v>
-      </c>
-      <c r="C99" s="82"/>
-      <c r="D99" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E99" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="83" t="s">
-        <v>736</v>
-      </c>
-      <c r="B100" s="80">
-        <v>696.0</v>
-      </c>
-      <c r="C100" s="82"/>
-      <c r="H100" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="83" t="s">
-        <v>738</v>
-      </c>
-      <c r="B101" s="80">
-        <v>695.0</v>
-      </c>
-      <c r="C101" s="82"/>
-      <c r="E101" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B102" s="80">
-        <v>674.0</v>
-      </c>
-      <c r="C102" s="82"/>
-      <c r="D102" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="83" t="s">
-        <v>740</v>
-      </c>
-      <c r="B103" s="80">
-        <v>653.0</v>
-      </c>
-      <c r="C103" s="82"/>
-      <c r="G103" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="80" t="s">
-        <v>228</v>
-      </c>
-      <c r="B104" s="80">
-        <v>603.0</v>
-      </c>
-      <c r="C104" s="82"/>
-      <c r="D104" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="83" t="s">
-        <v>742</v>
-      </c>
-      <c r="B105" s="80">
-        <v>598.0</v>
-      </c>
-      <c r="C105" s="82"/>
-      <c r="D105" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="83" t="s">
-        <v>744</v>
-      </c>
-      <c r="B106" s="80">
-        <v>588.0</v>
-      </c>
-      <c r="C106" s="82"/>
-      <c r="J106" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="85" t="s">
-        <v>746</v>
-      </c>
-      <c r="B107" s="80">
-        <v>588.0</v>
-      </c>
-      <c r="C107" s="82"/>
-      <c r="E107" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="83" t="s">
-        <v>748</v>
-      </c>
-      <c r="B108" s="80">
-        <v>565.0</v>
-      </c>
-      <c r="C108" s="82"/>
-      <c r="G108" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J108" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="83" t="s">
-        <v>750</v>
-      </c>
-      <c r="B109" s="80">
-        <v>561.0</v>
-      </c>
-      <c r="C109" s="82"/>
-      <c r="D109" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G109" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="80" t="s">
-        <v>818</v>
-      </c>
-      <c r="B110" s="80">
-        <v>546.0</v>
-      </c>
-      <c r="C110" s="82"/>
-      <c r="D110" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="80" t="s">
-        <v>819</v>
-      </c>
-      <c r="B111" s="80">
-        <v>502.0</v>
-      </c>
-      <c r="C111" s="81" t="s">
+      <c r="D136" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="137" ht="14.25" customHeight="1">
+      <c r="A137" s="81" t="s">
+        <v>829</v>
+      </c>
+      <c r="B137" s="81">
+        <v>226.0</v>
+      </c>
+      <c r="C137" s="83"/>
+      <c r="H137" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="138" ht="14.25" customHeight="1">
+      <c r="A138" s="81" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="81">
+        <v>221.0</v>
+      </c>
+      <c r="C138" s="83"/>
+      <c r="D138" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E138" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25" customHeight="1">
+      <c r="A139" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="B139" s="81">
+        <v>210.0</v>
+      </c>
+      <c r="C139" s="83"/>
+      <c r="I139" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="140" ht="14.25" customHeight="1">
+      <c r="A140" s="81" t="s">
+        <v>456</v>
+      </c>
+      <c r="B140" s="81">
+        <v>209.0</v>
+      </c>
+      <c r="C140" s="83"/>
+      <c r="H140" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="141" ht="14.25" customHeight="1">
+      <c r="A141" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="B141" s="81">
+        <v>181.0</v>
+      </c>
+      <c r="C141" s="83"/>
+      <c r="H141" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="142" ht="14.25" customHeight="1">
+      <c r="A142" s="81" t="s">
+        <v>466</v>
+      </c>
+      <c r="B142" s="81">
+        <v>175.0</v>
+      </c>
+      <c r="C142" s="83"/>
+      <c r="I142" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="143" ht="14.25" customHeight="1">
+      <c r="A143" s="81" t="s">
+        <v>597</v>
+      </c>
+      <c r="B143" s="81">
+        <v>151.0</v>
+      </c>
+      <c r="C143" s="83"/>
+      <c r="D143" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="144" ht="14.25" customHeight="1">
+      <c r="A144" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="B144" s="81">
+        <v>141.0</v>
+      </c>
+      <c r="C144" s="83"/>
+      <c r="D144" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="145" ht="14.25" customHeight="1">
+      <c r="A145" s="81" t="s">
+        <v>439</v>
+      </c>
+      <c r="B145" s="81">
+        <v>128.0</v>
+      </c>
+      <c r="C145" s="83"/>
+      <c r="H145" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="146" ht="14.25" customHeight="1">
+      <c r="A146" s="81" t="s">
+        <v>655</v>
+      </c>
+      <c r="B146" s="81">
+        <v>125.0</v>
+      </c>
+      <c r="C146" s="83"/>
+      <c r="H146" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="147" ht="14.25" customHeight="1">
+      <c r="A147" s="81" t="s">
+        <v>658</v>
+      </c>
+      <c r="B147" s="81">
+        <v>90.0</v>
+      </c>
+      <c r="C147" s="83"/>
+      <c r="D147" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E147" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="148" ht="14.25" customHeight="1">
+      <c r="A148" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B148" s="81">
+        <v>22.0</v>
+      </c>
+      <c r="C148" s="83"/>
+      <c r="E148" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="149" ht="14.25" customHeight="1">
+      <c r="A149" s="81" t="s">
+        <v>830</v>
+      </c>
+      <c r="B149" s="81">
+        <v>26.0</v>
+      </c>
+      <c r="C149" s="82" t="s">
+        <v>472</v>
+      </c>
+      <c r="H149" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="150" ht="14.25" customHeight="1">
+      <c r="A150" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="B150" s="81">
+        <v>29.0</v>
+      </c>
+      <c r="C150" s="83"/>
+      <c r="H150" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="151" ht="14.25" customHeight="1">
+      <c r="A151" s="81" t="s">
+        <v>831</v>
+      </c>
+      <c r="B151" s="81">
+        <v>34.0</v>
+      </c>
+      <c r="C151" s="83"/>
+      <c r="H151" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="152" ht="14.25" customHeight="1">
+      <c r="A152" s="81" t="s">
+        <v>542</v>
+      </c>
+      <c r="B152" s="81">
+        <v>35.0</v>
+      </c>
+      <c r="C152" s="83"/>
+      <c r="E152" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="153" ht="14.25" customHeight="1">
+      <c r="A153" s="81" t="s">
+        <v>583</v>
+      </c>
+      <c r="B153" s="81">
+        <v>61.0</v>
+      </c>
+      <c r="C153" s="83"/>
+      <c r="D153" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E153" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="154" ht="14.25" customHeight="1">
+      <c r="A154" s="81" t="s">
         <v>609</v>
       </c>
-      <c r="D111" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="83" t="s">
-        <v>753</v>
-      </c>
-      <c r="B112" s="80">
-        <v>480.0</v>
-      </c>
-      <c r="C112" s="82"/>
-      <c r="D112" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E112" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="80" t="s">
-        <v>409</v>
-      </c>
-      <c r="B113" s="80">
-        <v>473.0</v>
-      </c>
-      <c r="C113" s="82"/>
-    </row>
-    <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="80" t="s">
-        <v>820</v>
-      </c>
-      <c r="B114" s="80">
-        <v>432.0</v>
-      </c>
-      <c r="C114" s="81" t="s">
-        <v>528</v>
-      </c>
-      <c r="D114" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="80" t="s">
-        <v>821</v>
-      </c>
-      <c r="B115" s="80">
-        <v>424.0</v>
-      </c>
-      <c r="C115" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="D115" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="80" t="s">
-        <v>822</v>
-      </c>
-      <c r="B116" s="80">
-        <v>418.0</v>
-      </c>
-      <c r="C116" s="82"/>
-      <c r="D116" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="83" t="s">
-        <v>823</v>
-      </c>
-      <c r="B117" s="80">
-        <v>405.0</v>
-      </c>
-      <c r="C117" s="81" t="s">
-        <v>619</v>
-      </c>
-      <c r="D117" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J117" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="80" t="s">
-        <v>368</v>
-      </c>
-      <c r="B118" s="80">
-        <v>393.0</v>
-      </c>
-      <c r="C118" s="82"/>
-      <c r="H118" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="80" t="s">
-        <v>440</v>
-      </c>
-      <c r="B119" s="80">
-        <v>382.0</v>
-      </c>
-      <c r="C119" s="82"/>
-      <c r="D119" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="80" t="s">
-        <v>567</v>
-      </c>
-      <c r="B120" s="80">
-        <v>379.0</v>
-      </c>
-      <c r="C120" s="82"/>
-      <c r="H120" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="80" t="s">
-        <v>824</v>
-      </c>
-      <c r="B121" s="80">
-        <v>359.0</v>
-      </c>
-      <c r="C121" s="82"/>
-      <c r="H121" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="80" t="s">
-        <v>550</v>
-      </c>
-      <c r="B122" s="80">
-        <v>353.0</v>
-      </c>
-      <c r="C122" s="82"/>
-      <c r="D122" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="80" t="s">
-        <v>472</v>
-      </c>
-      <c r="B123" s="80">
-        <v>348.0</v>
-      </c>
-      <c r="C123" s="82"/>
-      <c r="H123" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="80" t="s">
-        <v>565</v>
-      </c>
-      <c r="B124" s="80">
-        <v>344.0</v>
-      </c>
-      <c r="C124" s="82"/>
-      <c r="D124" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="80" t="s">
-        <v>394</v>
-      </c>
-      <c r="B125" s="80">
-        <v>315.0</v>
-      </c>
-      <c r="C125" s="82"/>
-      <c r="D125" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="80" t="s">
-        <v>825</v>
-      </c>
-      <c r="B126" s="80">
-        <v>309.0</v>
-      </c>
-      <c r="C126" s="81" t="s">
-        <v>458</v>
-      </c>
-      <c r="D126" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="B127" s="80">
-        <v>283.0</v>
-      </c>
-      <c r="C127" s="82"/>
-      <c r="D127" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="80" t="s">
-        <v>826</v>
-      </c>
-      <c r="B128" s="80">
-        <v>279.0</v>
-      </c>
-      <c r="C128" s="81" t="s">
-        <v>84</v>
-      </c>
-      <c r="D128" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E128" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="80" t="s">
-        <v>503</v>
-      </c>
-      <c r="B129" s="80">
-        <v>278.0</v>
-      </c>
-      <c r="C129" s="82"/>
-      <c r="D129" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E129" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="80" t="s">
-        <v>827</v>
-      </c>
-      <c r="B130" s="80">
-        <v>276.0</v>
-      </c>
-      <c r="C130" s="81" t="s">
-        <v>253</v>
-      </c>
-      <c r="D130" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E130" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="80" t="s">
-        <v>182</v>
-      </c>
-      <c r="B131" s="80">
-        <v>274.0</v>
-      </c>
-      <c r="C131" s="82"/>
-      <c r="H131" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="80" t="s">
-        <v>828</v>
-      </c>
-      <c r="B132" s="80">
-        <v>264.0</v>
-      </c>
-      <c r="C132" s="82"/>
-      <c r="D132" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="80" t="s">
-        <v>270</v>
-      </c>
-      <c r="B133" s="80">
-        <v>262.0</v>
-      </c>
-      <c r="C133" s="82"/>
-      <c r="H133" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="80" t="s">
-        <v>829</v>
-      </c>
-      <c r="B134" s="80">
-        <v>250.0</v>
-      </c>
-      <c r="C134" s="82"/>
-      <c r="G134" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="B135" s="80">
-        <v>247.0</v>
-      </c>
-      <c r="C135" s="82"/>
-      <c r="E135" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="80" t="s">
-        <v>830</v>
-      </c>
-      <c r="B136" s="80">
-        <v>229.0</v>
-      </c>
-      <c r="C136" s="81" t="s">
-        <v>619</v>
-      </c>
-      <c r="D136" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="80" t="s">
-        <v>831</v>
-      </c>
-      <c r="B137" s="80">
-        <v>226.0</v>
-      </c>
-      <c r="C137" s="82"/>
-      <c r="H137" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="80" t="s">
-        <v>274</v>
-      </c>
-      <c r="B138" s="80">
-        <v>221.0</v>
-      </c>
-      <c r="C138" s="82"/>
-      <c r="D138" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E138" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="80" t="s">
-        <v>210</v>
-      </c>
-      <c r="B139" s="80">
-        <v>210.0</v>
-      </c>
-      <c r="C139" s="82"/>
-      <c r="I139" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="80" t="s">
-        <v>456</v>
-      </c>
-      <c r="B140" s="80">
-        <v>209.0</v>
-      </c>
-      <c r="C140" s="82"/>
-      <c r="H140" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="80" t="s">
-        <v>167</v>
-      </c>
-      <c r="B141" s="80">
-        <v>181.0</v>
-      </c>
-      <c r="C141" s="82"/>
-      <c r="H141" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="80" t="s">
-        <v>466</v>
-      </c>
-      <c r="B142" s="80">
-        <v>175.0</v>
-      </c>
-      <c r="C142" s="82"/>
-      <c r="I142" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="80" t="s">
-        <v>597</v>
-      </c>
-      <c r="B143" s="80">
-        <v>151.0</v>
-      </c>
-      <c r="C143" s="82"/>
-      <c r="D143" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="80" t="s">
-        <v>253</v>
-      </c>
-      <c r="B144" s="80">
-        <v>141.0</v>
-      </c>
-      <c r="C144" s="82"/>
-      <c r="D144" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" s="80" t="s">
-        <v>439</v>
-      </c>
-      <c r="B145" s="80">
-        <v>128.0</v>
-      </c>
-      <c r="C145" s="82"/>
-      <c r="H145" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="80" t="s">
-        <v>655</v>
-      </c>
-      <c r="B146" s="80">
-        <v>125.0</v>
-      </c>
-      <c r="C146" s="82"/>
-      <c r="H146" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" s="80" t="s">
-        <v>658</v>
-      </c>
-      <c r="B147" s="80">
-        <v>90.0</v>
-      </c>
-      <c r="C147" s="82"/>
-      <c r="D147" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E147" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="80" t="s">
-        <v>21</v>
-      </c>
-      <c r="B148" s="80">
-        <v>22.0</v>
-      </c>
-      <c r="C148" s="82"/>
-      <c r="E148" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="80" t="s">
+      <c r="B154" s="81">
+        <v>59.0</v>
+      </c>
+      <c r="C154" s="83"/>
+      <c r="H154" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="155" ht="14.25" customHeight="1">
+      <c r="A155" s="81" t="s">
         <v>832</v>
       </c>
-      <c r="B149" s="80">
-        <v>26.0</v>
-      </c>
-      <c r="C149" s="81" t="s">
-        <v>472</v>
-      </c>
-      <c r="H149" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="80" t="s">
-        <v>148</v>
-      </c>
-      <c r="B150" s="80">
-        <v>29.0</v>
-      </c>
-      <c r="C150" s="82"/>
-      <c r="H150" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="80" t="s">
-        <v>833</v>
-      </c>
-      <c r="B151" s="80">
-        <v>34.0</v>
-      </c>
-      <c r="C151" s="82"/>
-      <c r="H151" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="80" t="s">
-        <v>542</v>
-      </c>
-      <c r="B152" s="80">
-        <v>35.0</v>
-      </c>
-      <c r="C152" s="82"/>
-      <c r="E152" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="80" t="s">
-        <v>583</v>
-      </c>
-      <c r="B153" s="80">
-        <v>61.0</v>
-      </c>
-      <c r="C153" s="82"/>
-      <c r="D153" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E153" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="80" t="s">
-        <v>609</v>
-      </c>
-      <c r="B154" s="80">
-        <v>59.0</v>
-      </c>
-      <c r="C154" s="82"/>
-      <c r="H154" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="80" t="s">
-        <v>834</v>
-      </c>
-      <c r="B155" s="80">
+      <c r="B155" s="81">
         <v>74.0</v>
       </c>
-      <c r="C155" s="82"/>
+      <c r="C155" s="83"/>
       <c r="H155" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="80" t="s">
+      <c r="A156" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B156" s="80">
+      <c r="B156" s="81">
         <v>12.0</v>
       </c>
-      <c r="C156" s="82"/>
+      <c r="C156" s="83"/>
       <c r="H156" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="80" t="s">
+      <c r="A157" s="81" t="s">
         <v>256</v>
       </c>
-      <c r="B157" s="80">
+      <c r="B157" s="81">
         <v>80.0</v>
       </c>
-      <c r="C157" s="82"/>
+      <c r="C157" s="83"/>
       <c r="H157" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="80"/>
-      <c r="B158" s="80"/>
-      <c r="C158" s="82"/>
+      <c r="A158" s="81"/>
+      <c r="B158" s="81"/>
+      <c r="C158" s="83"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="84"/>
-      <c r="B159" s="84"/>
-      <c r="C159" s="82"/>
+      <c r="A159" s="85"/>
+      <c r="B159" s="85"/>
+      <c r="C159" s="83"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="84"/>
-      <c r="B160" s="84"/>
-      <c r="C160" s="82"/>
+      <c r="A160" s="85"/>
+      <c r="B160" s="85"/>
+      <c r="C160" s="83"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" s="84"/>
-      <c r="B161" s="84"/>
-      <c r="C161" s="82"/>
+      <c r="A161" s="85"/>
+      <c r="B161" s="85"/>
+      <c r="C161" s="83"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="84"/>
-      <c r="B162" s="84"/>
-      <c r="C162" s="82"/>
+      <c r="A162" s="85"/>
+      <c r="B162" s="85"/>
+      <c r="C162" s="83"/>
     </row>
     <row r="163" ht="14.25" customHeight="1"/>
     <row r="164" ht="14.25" customHeight="1"/>
@@ -31952,7 +31951,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>11</v>
@@ -32016,7 +32015,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>307</v>
@@ -32027,7 +32026,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>327</v>
@@ -32038,7 +32037,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>307</v>
@@ -32049,7 +32048,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>327</v>
@@ -32084,7 +32083,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
Corrected spelling misstakes in classLists
</commit_message>
<xml_diff>
--- a/GoogleOpenImages-allClasses.xlsx
+++ b/GoogleOpenImages-allClasses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="842">
   <si>
     <t>class</t>
   </si>
@@ -2382,6 +2382,9 @@
     <t>coffee maker</t>
   </si>
   <si>
+    <t>doorknob</t>
+  </si>
+  <si>
     <t>lightbulb</t>
   </si>
   <si>
@@ -2478,6 +2481,12 @@
     <t>chopping board</t>
   </si>
   <si>
+    <t>bow (decorative ribbons)</t>
+  </si>
+  <si>
+    <t>bow</t>
+  </si>
+  <si>
     <t>pot</t>
   </si>
   <si>
@@ -2502,7 +2511,7 @@
     <t>crate</t>
   </si>
   <si>
-    <t>pan</t>
+    <t>pan (for cooking)</t>
   </si>
   <si>
     <t>life jacket</t>
@@ -2545,7 +2554,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2686,6 +2695,10 @@
       <name val="Docs-Calibri"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2820,7 +2833,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3026,25 +3039,28 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3061,7 +3077,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -20606,8 +20622,8 @@
       <c r="D167" s="1">
         <v>30.0</v>
       </c>
-      <c r="E167" s="15" t="s">
-        <v>202</v>
+      <c r="E167" s="73" t="s">
+        <v>786</v>
       </c>
       <c r="F167" s="8">
         <v>1.0</v>
@@ -23224,7 +23240,7 @@
         <v>17.0</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F310" s="3">
         <v>1.0</v>
@@ -25431,7 +25447,7 @@
         <v>2.0</v>
       </c>
       <c r="E433" s="14" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F433" s="8">
         <v>1.0</v>
@@ -28543,11 +28559,11 @@
     </row>
     <row r="603" ht="14.25" customHeight="1"/>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="A604" s="73"/>
+      <c r="A604" s="74"/>
       <c r="D604" s="57"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="A605" s="74"/>
+      <c r="A605" s="75"/>
       <c r="D605" s="65"/>
     </row>
     <row r="606" ht="14.25" customHeight="1">
@@ -28555,23 +28571,23 @@
       <c r="D606" s="66"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="A607" s="73"/>
+      <c r="A607" s="74"/>
       <c r="D607" s="65"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="A608" s="73"/>
+      <c r="A608" s="74"/>
       <c r="D608" s="62"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="A609" s="73"/>
+      <c r="A609" s="74"/>
       <c r="D609" s="57"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="A610" s="73"/>
+      <c r="A610" s="74"/>
       <c r="D610" s="57"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="A611" s="75"/>
+      <c r="A611" s="76"/>
       <c r="D611" s="57"/>
     </row>
     <row r="612" ht="14.25" customHeight="1">
@@ -28579,38 +28595,38 @@
       <c r="D612" s="65"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="A613" s="73"/>
+      <c r="A613" s="74"/>
       <c r="D613" s="62"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="A614" s="76"/>
+      <c r="A614" s="77"/>
       <c r="D614" s="55"/>
     </row>
     <row r="615" ht="14.25" customHeight="1">
       <c r="D615" s="57"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="A616" s="76"/>
+      <c r="A616" s="77"/>
       <c r="D616" s="55"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="A617" s="77"/>
+      <c r="A617" s="78"/>
       <c r="D617" s="65"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="A618" s="73"/>
+      <c r="A618" s="74"/>
       <c r="D618" s="65"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="A619" s="73"/>
+      <c r="A619" s="74"/>
       <c r="D619" s="65"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="A620" s="77"/>
+      <c r="A620" s="78"/>
       <c r="D620" s="65"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="A621" s="73"/>
+      <c r="A621" s="74"/>
       <c r="D621" s="61"/>
     </row>
     <row r="622" ht="14.25" customHeight="1">
@@ -28625,11 +28641,11 @@
       <c r="D624" s="57"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="A625" s="78"/>
+      <c r="A625" s="79"/>
       <c r="D625" s="57"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="A626" s="79"/>
+      <c r="A626" s="80"/>
       <c r="D626" s="61"/>
     </row>
     <row r="627" ht="14.25" customHeight="1">
@@ -28646,16 +28662,16 @@
       <c r="D630" s="70"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="A631" s="75"/>
+      <c r="A631" s="76"/>
       <c r="D631" s="70"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="A632" s="78"/>
-      <c r="D632" s="80"/>
+      <c r="A632" s="79"/>
+      <c r="D632" s="81"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
       <c r="A633" s="69"/>
-      <c r="D633" s="80"/>
+      <c r="D633" s="81"/>
     </row>
     <row r="634" ht="14.25" customHeight="1"/>
     <row r="635" ht="14.25" customHeight="1"/>
@@ -29084,13 +29100,13 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="81" t="s">
-        <v>788</v>
-      </c>
-      <c r="B2" s="81">
+      <c r="A2" s="82" t="s">
+        <v>789</v>
+      </c>
+      <c r="B2" s="82">
         <v>164.0</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3">
@@ -29101,13 +29117,13 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="81" t="s">
-        <v>789</v>
-      </c>
-      <c r="B3" s="81">
+      <c r="A3" s="82" t="s">
+        <v>790</v>
+      </c>
+      <c r="B3" s="82">
         <v>2246.0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>481</v>
       </c>
       <c r="J3" s="3">
@@ -29115,91 +29131,91 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="82" t="s">
         <v>546</v>
       </c>
-      <c r="B4" s="81">
+      <c r="B4" s="82">
         <v>2231.0</v>
       </c>
-      <c r="C4" s="83"/>
+      <c r="C4" s="84"/>
       <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>531</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="82">
         <v>2216.0</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="84"/>
       <c r="J5" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="85" t="s">
         <v>685</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="82">
         <v>2215.0</v>
       </c>
-      <c r="C6" s="83"/>
+      <c r="C6" s="84"/>
       <c r="J6" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="82">
         <v>2214.0</v>
       </c>
-      <c r="C7" s="83"/>
+      <c r="C7" s="84"/>
       <c r="E7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="83"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="84"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="82" t="s">
         <v>455</v>
       </c>
-      <c r="B9" s="81">
+      <c r="B9" s="82">
         <v>2213.0</v>
       </c>
-      <c r="C9" s="83"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="81">
+      <c r="B10" s="82">
         <v>2203.0</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="84"/>
       <c r="E10" s="19"/>
       <c r="G10" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="82" t="s">
         <v>636</v>
       </c>
-      <c r="B11" s="81">
+      <c r="B11" s="82">
         <v>2203.0</v>
       </c>
-      <c r="C11" s="83"/>
+      <c r="C11" s="84"/>
       <c r="E11" s="3">
         <v>1.0</v>
       </c>
@@ -29208,25 +29224,25 @@
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="82" t="s">
         <v>653</v>
       </c>
-      <c r="B12" s="81">
+      <c r="B12" s="82">
         <v>2193.0</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="84"/>
       <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="81">
+      <c r="B13" s="82">
         <v>2182.0</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="3">
         <v>1.0</v>
       </c>
@@ -29238,13 +29254,13 @@
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="81" t="s">
-        <v>790</v>
-      </c>
-      <c r="B14" s="81">
+      <c r="A14" s="82" t="s">
+        <v>791</v>
+      </c>
+      <c r="B14" s="82">
         <v>2190.0</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="83" t="s">
         <v>171</v>
       </c>
       <c r="D14" s="3">
@@ -29252,111 +29268,111 @@
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="84" t="s">
-        <v>791</v>
-      </c>
-      <c r="B15" s="81">
+      <c r="A15" s="85" t="s">
+        <v>792</v>
+      </c>
+      <c r="B15" s="82">
         <v>2188.0</v>
       </c>
-      <c r="C15" s="82" t="s">
-        <v>792</v>
+      <c r="C15" s="83" t="s">
+        <v>793</v>
       </c>
       <c r="D15" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="82" t="s">
         <v>242</v>
       </c>
-      <c r="B16" s="81">
+      <c r="B16" s="82">
         <v>2182.0</v>
       </c>
-      <c r="C16" s="83"/>
+      <c r="C16" s="84"/>
       <c r="G16" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="85" t="s">
         <v>694</v>
       </c>
-      <c r="B17" s="81">
+      <c r="B17" s="82">
         <v>2178.0</v>
       </c>
-      <c r="C17" s="83"/>
+      <c r="C17" s="84"/>
       <c r="G17" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="82" t="s">
         <v>525</v>
       </c>
-      <c r="B18" s="81">
+      <c r="B18" s="82">
         <v>2174.0</v>
       </c>
-      <c r="C18" s="83"/>
+      <c r="C18" s="84"/>
       <c r="G18" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="82" t="s">
         <v>532</v>
       </c>
-      <c r="B19" s="81">
+      <c r="B19" s="82">
         <v>2171.0</v>
       </c>
-      <c r="C19" s="83"/>
+      <c r="C19" s="84"/>
       <c r="J19" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="82" t="s">
         <v>413</v>
       </c>
-      <c r="B20" s="81">
+      <c r="B20" s="82">
         <v>2167.0</v>
       </c>
-      <c r="C20" s="83"/>
+      <c r="C20" s="84"/>
       <c r="G20" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="81">
+      <c r="B21" s="82">
         <v>2163.0</v>
       </c>
-      <c r="C21" s="83"/>
+      <c r="C21" s="84"/>
       <c r="D21" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="82" t="s">
         <v>459</v>
       </c>
-      <c r="B22" s="81">
+      <c r="B22" s="82">
         <v>2163.0</v>
       </c>
-      <c r="C22" s="83"/>
+      <c r="C22" s="84"/>
       <c r="H22" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="81" t="s">
-        <v>793</v>
-      </c>
-      <c r="B23" s="81">
+      <c r="A23" s="82" t="s">
+        <v>794</v>
+      </c>
+      <c r="B23" s="82">
         <v>2162.0</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="83" t="s">
         <v>593</v>
       </c>
       <c r="D23" s="3">
@@ -29364,25 +29380,25 @@
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="B24" s="81">
+      <c r="B24" s="82">
         <v>2157.0</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="84"/>
       <c r="D24" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="85" t="s">
         <v>698</v>
       </c>
-      <c r="B25" s="81">
+      <c r="B25" s="82">
         <v>2155.0</v>
       </c>
-      <c r="C25" s="83"/>
+      <c r="C25" s="84"/>
       <c r="D25" s="3">
         <v>1.0</v>
       </c>
@@ -29391,205 +29407,205 @@
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="82" t="s">
         <v>262</v>
       </c>
-      <c r="B26" s="81">
+      <c r="B26" s="82">
         <v>2152.0</v>
       </c>
-      <c r="C26" s="83"/>
+      <c r="C26" s="84"/>
       <c r="G26" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="81" t="s">
-        <v>794</v>
-      </c>
-      <c r="B27" s="81">
+      <c r="A27" s="82" t="s">
+        <v>795</v>
+      </c>
+      <c r="B27" s="82">
         <v>2152.0</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="84"/>
       <c r="D27" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="82" t="s">
         <v>639</v>
       </c>
-      <c r="B28" s="81">
+      <c r="B28" s="82">
         <v>2138.0</v>
       </c>
-      <c r="C28" s="83"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="81">
+      <c r="B29" s="82">
         <v>2140.0</v>
       </c>
-      <c r="C29" s="83"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="81" t="s">
-        <v>795</v>
-      </c>
-      <c r="B30" s="81">
+      <c r="A30" s="82" t="s">
+        <v>796</v>
+      </c>
+      <c r="B30" s="82">
         <v>2133.0</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="84"/>
       <c r="G30" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="82" t="s">
         <v>398</v>
       </c>
-      <c r="B31" s="81">
+      <c r="B31" s="82">
         <v>2132.0</v>
       </c>
-      <c r="C31" s="83"/>
+      <c r="C31" s="84"/>
       <c r="D31" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="84" t="s">
-        <v>796</v>
-      </c>
-      <c r="B32" s="81">
+      <c r="A32" s="85" t="s">
+        <v>797</v>
+      </c>
+      <c r="B32" s="82">
         <v>2129.0</v>
       </c>
-      <c r="C32" s="83"/>
+      <c r="C32" s="84"/>
       <c r="E32" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="82" t="s">
         <v>577</v>
       </c>
-      <c r="B33" s="81">
+      <c r="B33" s="82">
         <v>2127.0</v>
       </c>
-      <c r="C33" s="83"/>
+      <c r="C33" s="84"/>
       <c r="J33" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="82" t="s">
         <v>355</v>
       </c>
-      <c r="B34" s="81">
+      <c r="B34" s="82">
         <v>2125.0</v>
       </c>
-      <c r="C34" s="83"/>
+      <c r="C34" s="84"/>
       <c r="D34" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="B35" s="81">
+      <c r="B35" s="82">
         <v>2115.0</v>
       </c>
-      <c r="C35" s="83"/>
+      <c r="C35" s="84"/>
       <c r="I35" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="B36" s="81">
+      <c r="B36" s="82">
         <v>2114.0</v>
       </c>
-      <c r="C36" s="83"/>
+      <c r="C36" s="84"/>
       <c r="D36" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="B37" s="81">
+      <c r="B37" s="82">
         <v>2113.0</v>
       </c>
-      <c r="C37" s="83"/>
+      <c r="C37" s="84"/>
       <c r="I37" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="81">
+      <c r="B38" s="82">
         <v>2106.0</v>
       </c>
-      <c r="C38" s="83"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="84" t="s">
+      <c r="A39" s="85" t="s">
         <v>703</v>
       </c>
-      <c r="B39" s="81">
+      <c r="B39" s="82">
         <v>2088.0</v>
       </c>
-      <c r="C39" s="83"/>
+      <c r="C39" s="84"/>
       <c r="G39" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="82" t="s">
         <v>363</v>
       </c>
-      <c r="B40" s="81">
+      <c r="B40" s="82">
         <v>2067.0</v>
       </c>
-      <c r="C40" s="83"/>
+      <c r="C40" s="84"/>
       <c r="D40" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="81">
+      <c r="B41" s="82">
         <v>1997.0</v>
       </c>
-      <c r="C41" s="83"/>
+      <c r="C41" s="84"/>
       <c r="H41" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="81">
+      <c r="B42" s="82">
         <v>1997.0</v>
       </c>
-      <c r="C42" s="83"/>
+      <c r="C42" s="84"/>
       <c r="D42" s="3">
         <v>1.0</v>
       </c>
@@ -29598,25 +29614,25 @@
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="81" t="s">
-        <v>797</v>
-      </c>
-      <c r="B43" s="81">
+      <c r="A43" s="82" t="s">
+        <v>798</v>
+      </c>
+      <c r="B43" s="82">
         <v>1995.0</v>
       </c>
-      <c r="C43" s="83"/>
+      <c r="C43" s="84"/>
       <c r="J43" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="84" t="s">
-        <v>202</v>
-      </c>
-      <c r="B44" s="81">
+      <c r="A44" s="85" t="s">
+        <v>786</v>
+      </c>
+      <c r="B44" s="82">
         <v>1948.0</v>
       </c>
-      <c r="C44" s="83"/>
+      <c r="C44" s="84"/>
       <c r="D44" s="3">
         <v>1.0</v>
       </c>
@@ -29625,61 +29641,61 @@
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="81" t="s">
-        <v>798</v>
-      </c>
-      <c r="B45" s="81">
+      <c r="A45" s="82" t="s">
+        <v>799</v>
+      </c>
+      <c r="B45" s="82">
         <v>1920.0</v>
       </c>
-      <c r="C45" s="83"/>
+      <c r="C45" s="84"/>
       <c r="D45" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="82" t="s">
         <v>675</v>
       </c>
-      <c r="B46" s="81">
+      <c r="B46" s="82">
         <v>1902.0</v>
       </c>
-      <c r="C46" s="83"/>
+      <c r="C46" s="84"/>
       <c r="I46" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="84" t="s">
+      <c r="A47" s="85" t="s">
         <v>710</v>
       </c>
-      <c r="B47" s="81">
+      <c r="B47" s="82">
         <v>1877.0</v>
       </c>
-      <c r="C47" s="83"/>
+      <c r="C47" s="84"/>
       <c r="G47" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="82" t="s">
         <v>530</v>
       </c>
-      <c r="B48" s="81">
+      <c r="B48" s="82">
         <v>1869.0</v>
       </c>
-      <c r="C48" s="83"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="82" t="s">
         <v>574</v>
       </c>
-      <c r="B49" s="81">
+      <c r="B49" s="82">
         <v>1831.0</v>
       </c>
-      <c r="C49" s="83"/>
+      <c r="C49" s="84"/>
       <c r="D49" s="3">
         <v>1.0</v>
       </c>
@@ -29688,85 +29704,85 @@
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="84" t="s">
-        <v>799</v>
-      </c>
-      <c r="B50" s="81">
+      <c r="A50" s="85" t="s">
+        <v>800</v>
+      </c>
+      <c r="B50" s="82">
         <v>1784.0</v>
       </c>
-      <c r="C50" s="83"/>
+      <c r="C50" s="84"/>
       <c r="G50" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="81">
+      <c r="B51" s="82">
         <v>1709.0</v>
       </c>
-      <c r="C51" s="83"/>
+      <c r="C51" s="84"/>
       <c r="H51" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="82" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="81">
+      <c r="B52" s="82">
         <v>1698.0</v>
       </c>
-      <c r="C52" s="83"/>
+      <c r="C52" s="84"/>
       <c r="D52" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="82" t="s">
         <v>206</v>
       </c>
-      <c r="B53" s="81">
+      <c r="B53" s="82">
         <v>1664.0</v>
       </c>
-      <c r="C53" s="83"/>
+      <c r="C53" s="84"/>
       <c r="G53" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="82" t="s">
         <v>487</v>
       </c>
-      <c r="B54" s="81">
+      <c r="B54" s="82">
         <v>1655.0</v>
       </c>
-      <c r="C54" s="83"/>
+      <c r="C54" s="84"/>
       <c r="D54" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="81" t="s">
-        <v>800</v>
-      </c>
-      <c r="B55" s="81">
+      <c r="A55" s="82" t="s">
+        <v>801</v>
+      </c>
+      <c r="B55" s="82">
         <v>1640.0</v>
       </c>
-      <c r="C55" s="83"/>
+      <c r="C55" s="84"/>
       <c r="D55" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="84" t="s">
-        <v>801</v>
-      </c>
-      <c r="B56" s="81">
+      <c r="A56" s="85" t="s">
+        <v>802</v>
+      </c>
+      <c r="B56" s="82">
         <v>1639.0</v>
       </c>
-      <c r="C56" s="83"/>
+      <c r="C56" s="84"/>
       <c r="G56" s="3">
         <v>1.0</v>
       </c>
@@ -29775,197 +29791,197 @@
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="81" t="s">
+      <c r="A57" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="81">
+      <c r="B57" s="82">
         <v>1611.0</v>
       </c>
-      <c r="C57" s="83"/>
+      <c r="C57" s="84"/>
       <c r="I57" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="81">
+      <c r="B58" s="82">
         <v>1578.0</v>
       </c>
-      <c r="C58" s="83"/>
+      <c r="C58" s="84"/>
       <c r="G58" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="81">
+      <c r="B59" s="82">
         <v>1520.0</v>
       </c>
-      <c r="C59" s="83"/>
+      <c r="C59" s="84"/>
       <c r="H59" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="81" t="s">
-        <v>802</v>
-      </c>
-      <c r="B60" s="81">
+      <c r="A60" s="82" t="s">
+        <v>803</v>
+      </c>
+      <c r="B60" s="82">
         <v>1482.0</v>
       </c>
-      <c r="C60" s="83"/>
+      <c r="C60" s="84"/>
       <c r="J60" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="81" t="s">
-        <v>803</v>
-      </c>
-      <c r="B61" s="81">
+      <c r="A61" s="82" t="s">
+        <v>804</v>
+      </c>
+      <c r="B61" s="82">
         <v>1383.0</v>
       </c>
-      <c r="C61" s="83"/>
+      <c r="C61" s="84"/>
       <c r="H61" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="81" t="s">
+      <c r="A62" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="81">
+      <c r="B62" s="82">
         <v>1382.0</v>
       </c>
-      <c r="C62" s="83"/>
+      <c r="C62" s="84"/>
       <c r="H62" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="81" t="s">
+      <c r="A63" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="81">
+      <c r="B63" s="82">
         <v>1339.0</v>
       </c>
-      <c r="C63" s="83"/>
+      <c r="C63" s="84"/>
       <c r="H63" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="81" t="s">
+      <c r="A64" s="82" t="s">
         <v>553</v>
       </c>
-      <c r="B64" s="81">
+      <c r="B64" s="82">
         <v>1287.0</v>
       </c>
-      <c r="C64" s="83"/>
+      <c r="C64" s="84"/>
       <c r="D64" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="81" t="s">
-        <v>804</v>
-      </c>
-      <c r="B65" s="81">
+      <c r="A65" s="82" t="s">
+        <v>805</v>
+      </c>
+      <c r="B65" s="82">
         <v>1273.0</v>
       </c>
-      <c r="C65" s="83"/>
+      <c r="C65" s="84"/>
       <c r="D65" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="81" t="s">
+      <c r="A66" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="B66" s="81">
+      <c r="B66" s="82">
         <v>1257.0</v>
       </c>
-      <c r="C66" s="83"/>
+      <c r="C66" s="84"/>
       <c r="D66" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="84" t="s">
+      <c r="A67" s="85" t="s">
         <v>723</v>
       </c>
-      <c r="B67" s="81">
+      <c r="B67" s="82">
         <v>1247.0</v>
       </c>
-      <c r="C67" s="83"/>
+      <c r="C67" s="84"/>
       <c r="E67" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="86" t="s">
-        <v>805</v>
-      </c>
-      <c r="B68" s="81">
+      <c r="A68" s="87" t="s">
+        <v>806</v>
+      </c>
+      <c r="B68" s="82">
         <v>1227.0</v>
       </c>
-      <c r="C68" s="83"/>
+      <c r="C68" s="84"/>
       <c r="G68" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="81" t="s">
+      <c r="A69" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="B69" s="81">
+      <c r="B69" s="82">
         <v>1170.0</v>
       </c>
-      <c r="C69" s="83"/>
+      <c r="C69" s="84"/>
       <c r="D69" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="81" t="s">
-        <v>806</v>
-      </c>
-      <c r="B70" s="81">
+      <c r="A70" s="82" t="s">
+        <v>807</v>
+      </c>
+      <c r="B70" s="82">
         <v>1164.0</v>
       </c>
-      <c r="C70" s="82" t="s">
-        <v>807</v>
+      <c r="C70" s="83" t="s">
+        <v>808</v>
       </c>
       <c r="D70" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="84" t="s">
+      <c r="A71" s="85" t="s">
         <v>728</v>
       </c>
-      <c r="B71" s="81">
+      <c r="B71" s="82">
         <v>1130.0</v>
       </c>
-      <c r="C71" s="82" t="s">
-        <v>808</v>
+      <c r="C71" s="83" t="s">
+        <v>809</v>
       </c>
       <c r="D71" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="81" t="s">
-        <v>809</v>
-      </c>
-      <c r="B72" s="81">
+      <c r="A72" s="82" t="s">
+        <v>810</v>
+      </c>
+      <c r="B72" s="82">
         <v>1129.0</v>
       </c>
-      <c r="C72" s="83"/>
+      <c r="C72" s="84"/>
       <c r="E72" s="3">
         <v>1.0</v>
       </c>
@@ -29974,109 +29990,109 @@
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="81" t="s">
-        <v>810</v>
-      </c>
-      <c r="B73" s="81">
+      <c r="A73" s="82" t="s">
+        <v>811</v>
+      </c>
+      <c r="B73" s="82">
         <v>1124.0</v>
       </c>
-      <c r="C73" s="83"/>
+      <c r="C73" s="84"/>
       <c r="G73" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="81" t="s">
+      <c r="A74" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="B74" s="81">
+      <c r="B74" s="82">
         <v>1102.0</v>
       </c>
-      <c r="C74" s="83"/>
+      <c r="C74" s="84"/>
       <c r="H74" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="81" t="s">
-        <v>811</v>
-      </c>
-      <c r="B75" s="81">
+      <c r="A75" s="82" t="s">
+        <v>812</v>
+      </c>
+      <c r="B75" s="82">
         <v>1097.0</v>
       </c>
-      <c r="C75" s="83"/>
+      <c r="C75" s="84"/>
       <c r="D75" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="84" t="s">
+      <c r="A76" s="85" t="s">
         <v>729</v>
       </c>
-      <c r="B76" s="81">
+      <c r="B76" s="82">
         <v>1089.0</v>
       </c>
-      <c r="C76" s="83"/>
+      <c r="C76" s="84"/>
       <c r="G76" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="81" t="s">
+      <c r="A77" s="82" t="s">
         <v>522</v>
       </c>
-      <c r="B77" s="81">
+      <c r="B77" s="82">
         <v>1075.0</v>
       </c>
-      <c r="C77" s="83"/>
+      <c r="C77" s="84"/>
       <c r="I77" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="81" t="s">
+      <c r="A78" s="82" t="s">
         <v>519</v>
       </c>
-      <c r="B78" s="81">
+      <c r="B78" s="82">
         <v>1033.0</v>
       </c>
-      <c r="C78" s="83"/>
+      <c r="C78" s="84"/>
       <c r="D78" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="81" t="s">
-        <v>786</v>
-      </c>
-      <c r="B79" s="81">
+      <c r="A79" s="82" t="s">
+        <v>787</v>
+      </c>
+      <c r="B79" s="82">
         <v>991.0</v>
       </c>
-      <c r="C79" s="83"/>
+      <c r="C79" s="84"/>
       <c r="D79" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="84" t="s">
+      <c r="A80" s="85" t="s">
         <v>730</v>
       </c>
-      <c r="B80" s="81">
+      <c r="B80" s="82">
         <v>978.0</v>
       </c>
-      <c r="C80" s="83"/>
+      <c r="C80" s="84"/>
       <c r="G80" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="81" t="s">
+      <c r="A81" s="82" t="s">
         <v>407</v>
       </c>
-      <c r="B81" s="81">
+      <c r="B81" s="82">
         <v>933.0</v>
       </c>
-      <c r="C81" s="82" t="s">
+      <c r="C81" s="83" t="s">
         <v>151</v>
       </c>
       <c r="D81" s="3">
@@ -30084,109 +30100,109 @@
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="81" t="s">
+      <c r="A82" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B82" s="81">
+      <c r="B82" s="82">
         <v>929.0</v>
       </c>
-      <c r="C82" s="83"/>
+      <c r="C82" s="84"/>
       <c r="D82" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="81" t="s">
-        <v>812</v>
-      </c>
-      <c r="B83" s="81">
+      <c r="A83" s="82" t="s">
+        <v>813</v>
+      </c>
+      <c r="B83" s="82">
         <v>921.0</v>
       </c>
-      <c r="C83" s="83"/>
+      <c r="C83" s="84"/>
       <c r="H83" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="81" t="s">
+      <c r="A84" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="B84" s="81">
+      <c r="B84" s="82">
         <v>918.0</v>
       </c>
-      <c r="C84" s="83"/>
+      <c r="C84" s="84"/>
       <c r="H84" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="81" t="s">
-        <v>813</v>
-      </c>
-      <c r="B85" s="81">
+      <c r="A85" s="82" t="s">
+        <v>814</v>
+      </c>
+      <c r="B85" s="82">
         <v>892.0</v>
       </c>
-      <c r="C85" s="83"/>
+      <c r="C85" s="84"/>
       <c r="G85" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="88" t="s">
         <v>506</v>
       </c>
-      <c r="B86" s="81">
+      <c r="B86" s="82">
         <v>863.0</v>
       </c>
-      <c r="C86" s="83"/>
+      <c r="C86" s="84"/>
       <c r="G86" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="81" t="s">
+      <c r="A87" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="B87" s="81">
+      <c r="B87" s="82">
         <v>831.0</v>
       </c>
-      <c r="C87" s="83"/>
+      <c r="C87" s="84"/>
       <c r="G87" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="81" t="s">
+      <c r="A88" s="82" t="s">
         <v>616</v>
       </c>
-      <c r="B88" s="81">
+      <c r="B88" s="82">
         <v>831.0</v>
       </c>
-      <c r="C88" s="83"/>
+      <c r="C88" s="84"/>
       <c r="D88" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="81" t="s">
+      <c r="A89" s="82" t="s">
         <v>507</v>
       </c>
-      <c r="B89" s="81">
+      <c r="B89" s="82">
         <v>804.0</v>
       </c>
-      <c r="C89" s="83"/>
+      <c r="C89" s="84"/>
       <c r="D89" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="84" t="s">
+      <c r="A90" s="85" t="s">
         <v>731</v>
       </c>
-      <c r="B90" s="81">
+      <c r="B90" s="82">
         <v>801.0</v>
       </c>
-      <c r="C90" s="83"/>
+      <c r="C90" s="84"/>
       <c r="D90" s="3">
         <v>1.0</v>
       </c>
@@ -30195,37 +30211,37 @@
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="81" t="s">
+      <c r="A91" s="82" t="s">
         <v>423</v>
       </c>
-      <c r="B91" s="81">
+      <c r="B91" s="82">
         <v>776.0</v>
       </c>
-      <c r="C91" s="83"/>
+      <c r="C91" s="84"/>
       <c r="D91" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="84" t="s">
-        <v>814</v>
-      </c>
-      <c r="B92" s="81">
+      <c r="A92" s="85" t="s">
+        <v>815</v>
+      </c>
+      <c r="B92" s="82">
         <v>772.0</v>
       </c>
-      <c r="C92" s="83"/>
+      <c r="C92" s="84"/>
       <c r="G92" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="81" t="s">
-        <v>815</v>
-      </c>
-      <c r="B93" s="81">
+      <c r="A93" s="82" t="s">
+        <v>816</v>
+      </c>
+      <c r="B93" s="82">
         <v>770.0</v>
       </c>
-      <c r="C93" s="82" t="s">
+      <c r="C93" s="83" t="s">
         <v>498</v>
       </c>
       <c r="H93" s="3">
@@ -30233,61 +30249,61 @@
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="81" t="s">
-        <v>816</v>
-      </c>
-      <c r="B94" s="81">
+      <c r="A94" s="82" t="s">
+        <v>817</v>
+      </c>
+      <c r="B94" s="82">
         <v>739.0</v>
       </c>
-      <c r="C94" s="83"/>
+      <c r="C94" s="84"/>
       <c r="H94" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="81" t="s">
+      <c r="A95" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B95" s="81">
+      <c r="B95" s="82">
         <v>735.0</v>
       </c>
-      <c r="C95" s="83"/>
+      <c r="C95" s="84"/>
       <c r="I95" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="81" t="s">
-        <v>817</v>
-      </c>
-      <c r="B96" s="81">
+      <c r="A96" s="82" t="s">
+        <v>818</v>
+      </c>
+      <c r="B96" s="82">
         <v>732.0</v>
       </c>
-      <c r="C96" s="83"/>
+      <c r="C96" s="84"/>
       <c r="D96" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="84" t="s">
+      <c r="A97" s="85" t="s">
         <v>734</v>
       </c>
-      <c r="B97" s="81">
+      <c r="B97" s="82">
         <v>727.0</v>
       </c>
-      <c r="C97" s="83"/>
+      <c r="C97" s="84"/>
       <c r="E97" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="81" t="s">
+      <c r="A98" s="82" t="s">
         <v>619</v>
       </c>
-      <c r="B98" s="81">
+      <c r="B98" s="82">
         <v>719.0</v>
       </c>
-      <c r="C98" s="83"/>
+      <c r="C98" s="84"/>
       <c r="D98" s="3">
         <v>1.0</v>
       </c>
@@ -30296,13 +30312,13 @@
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="81" t="s">
+      <c r="A99" s="82" t="s">
         <v>360</v>
       </c>
-      <c r="B99" s="81">
+      <c r="B99" s="82">
         <v>710.0</v>
       </c>
-      <c r="C99" s="83"/>
+      <c r="C99" s="84"/>
       <c r="D99" s="3">
         <v>1.0</v>
       </c>
@@ -30311,109 +30327,109 @@
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="84" t="s">
+      <c r="A100" s="85" t="s">
         <v>736</v>
       </c>
-      <c r="B100" s="81">
+      <c r="B100" s="82">
         <v>696.0</v>
       </c>
-      <c r="C100" s="83"/>
+      <c r="C100" s="84"/>
       <c r="H100" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="84" t="s">
+      <c r="A101" s="85" t="s">
         <v>738</v>
       </c>
-      <c r="B101" s="81">
+      <c r="B101" s="82">
         <v>695.0</v>
       </c>
-      <c r="C101" s="83"/>
+      <c r="C101" s="84"/>
       <c r="E101" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="81" t="s">
+      <c r="A102" s="82" t="s">
         <v>127</v>
       </c>
-      <c r="B102" s="81">
+      <c r="B102" s="82">
         <v>674.0</v>
       </c>
-      <c r="C102" s="83"/>
+      <c r="C102" s="84"/>
       <c r="D102" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="84" t="s">
+      <c r="A103" s="85" t="s">
         <v>740</v>
       </c>
-      <c r="B103" s="81">
+      <c r="B103" s="82">
         <v>653.0</v>
       </c>
-      <c r="C103" s="83"/>
+      <c r="C103" s="84"/>
       <c r="G103" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="81" t="s">
+      <c r="A104" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="B104" s="81">
+      <c r="B104" s="82">
         <v>603.0</v>
       </c>
-      <c r="C104" s="83"/>
+      <c r="C104" s="84"/>
       <c r="D104" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="84" t="s">
+      <c r="A105" s="85" t="s">
         <v>742</v>
       </c>
-      <c r="B105" s="81">
+      <c r="B105" s="82">
         <v>598.0</v>
       </c>
-      <c r="C105" s="83"/>
+      <c r="C105" s="84"/>
       <c r="D105" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="84" t="s">
+      <c r="A106" s="85" t="s">
         <v>744</v>
       </c>
-      <c r="B106" s="81">
+      <c r="B106" s="82">
         <v>588.0</v>
       </c>
-      <c r="C106" s="83"/>
+      <c r="C106" s="84"/>
       <c r="J106" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="86" t="s">
+      <c r="A107" s="87" t="s">
         <v>746</v>
       </c>
-      <c r="B107" s="81">
+      <c r="B107" s="82">
         <v>588.0</v>
       </c>
-      <c r="C107" s="83"/>
+      <c r="C107" s="84"/>
       <c r="E107" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="84" t="s">
+      <c r="A108" s="85" t="s">
         <v>748</v>
       </c>
-      <c r="B108" s="81">
+      <c r="B108" s="82">
         <v>565.0</v>
       </c>
-      <c r="C108" s="83"/>
+      <c r="C108" s="84"/>
       <c r="G108" s="3">
         <v>1.0</v>
       </c>
@@ -30422,13 +30438,15 @@
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="84" t="s">
-        <v>750</v>
-      </c>
-      <c r="B109" s="81">
+      <c r="A109" s="85" t="s">
+        <v>819</v>
+      </c>
+      <c r="B109" s="82">
         <v>561.0</v>
       </c>
-      <c r="C109" s="83"/>
+      <c r="C109" s="83" t="s">
+        <v>820</v>
+      </c>
       <c r="D109" s="3">
         <v>1.0</v>
       </c>
@@ -30437,25 +30455,25 @@
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="81" t="s">
-        <v>818</v>
-      </c>
-      <c r="B110" s="81">
+      <c r="A110" s="82" t="s">
+        <v>821</v>
+      </c>
+      <c r="B110" s="82">
         <v>546.0</v>
       </c>
-      <c r="C110" s="83"/>
+      <c r="C110" s="84"/>
       <c r="D110" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="81" t="s">
-        <v>819</v>
-      </c>
-      <c r="B111" s="81">
+      <c r="A111" s="82" t="s">
+        <v>822</v>
+      </c>
+      <c r="B111" s="82">
         <v>502.0</v>
       </c>
-      <c r="C111" s="82" t="s">
+      <c r="C111" s="83" t="s">
         <v>609</v>
       </c>
       <c r="D111" s="3">
@@ -30463,13 +30481,13 @@
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="84" t="s">
+      <c r="A112" s="85" t="s">
         <v>753</v>
       </c>
-      <c r="B112" s="81">
+      <c r="B112" s="82">
         <v>480.0</v>
       </c>
-      <c r="C112" s="83"/>
+      <c r="C112" s="84"/>
       <c r="D112" s="3">
         <v>1.0</v>
       </c>
@@ -30478,22 +30496,22 @@
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="81" t="s">
+      <c r="A113" s="82" t="s">
         <v>409</v>
       </c>
-      <c r="B113" s="81">
+      <c r="B113" s="82">
         <v>473.0</v>
       </c>
-      <c r="C113" s="83"/>
+      <c r="C113" s="84"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="81" t="s">
-        <v>820</v>
-      </c>
-      <c r="B114" s="81">
+      <c r="A114" s="82" t="s">
+        <v>823</v>
+      </c>
+      <c r="B114" s="82">
         <v>432.0</v>
       </c>
-      <c r="C114" s="82" t="s">
+      <c r="C114" s="83" t="s">
         <v>528</v>
       </c>
       <c r="D114" s="3">
@@ -30501,13 +30519,13 @@
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="81" t="s">
-        <v>821</v>
-      </c>
-      <c r="B115" s="81">
+      <c r="A115" s="82" t="s">
+        <v>824</v>
+      </c>
+      <c r="B115" s="82">
         <v>424.0</v>
       </c>
-      <c r="C115" s="82" t="s">
+      <c r="C115" s="83" t="s">
         <v>183</v>
       </c>
       <c r="D115" s="3">
@@ -30515,25 +30533,27 @@
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="81" t="s">
-        <v>787</v>
-      </c>
-      <c r="B116" s="81">
+      <c r="A116" s="82" t="s">
+        <v>500</v>
+      </c>
+      <c r="B116" s="82">
         <v>418.0</v>
       </c>
-      <c r="C116" s="83"/>
+      <c r="C116" s="83" t="s">
+        <v>788</v>
+      </c>
       <c r="D116" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="84" t="s">
-        <v>822</v>
-      </c>
-      <c r="B117" s="81">
+      <c r="A117" s="85" t="s">
+        <v>825</v>
+      </c>
+      <c r="B117" s="82">
         <v>405.0</v>
       </c>
-      <c r="C117" s="82" t="s">
+      <c r="C117" s="83" t="s">
         <v>619</v>
       </c>
       <c r="D117" s="3">
@@ -30544,109 +30564,109 @@
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="81" t="s">
+      <c r="A118" s="82" t="s">
         <v>368</v>
       </c>
-      <c r="B118" s="81">
+      <c r="B118" s="82">
         <v>393.0</v>
       </c>
-      <c r="C118" s="83"/>
+      <c r="C118" s="84"/>
       <c r="H118" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="81" t="s">
+      <c r="A119" s="82" t="s">
         <v>440</v>
       </c>
-      <c r="B119" s="81">
+      <c r="B119" s="82">
         <v>382.0</v>
       </c>
-      <c r="C119" s="83"/>
+      <c r="C119" s="84"/>
       <c r="D119" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="81" t="s">
+      <c r="A120" s="82" t="s">
         <v>567</v>
       </c>
-      <c r="B120" s="81">
+      <c r="B120" s="82">
         <v>379.0</v>
       </c>
-      <c r="C120" s="83"/>
+      <c r="C120" s="84"/>
       <c r="H120" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="81" t="s">
-        <v>823</v>
-      </c>
-      <c r="B121" s="81">
+      <c r="A121" s="82" t="s">
+        <v>826</v>
+      </c>
+      <c r="B121" s="82">
         <v>359.0</v>
       </c>
-      <c r="C121" s="83"/>
+      <c r="C121" s="84"/>
       <c r="H121" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="81" t="s">
+      <c r="A122" s="82" t="s">
         <v>550</v>
       </c>
-      <c r="B122" s="81">
+      <c r="B122" s="82">
         <v>353.0</v>
       </c>
-      <c r="C122" s="83"/>
+      <c r="C122" s="84"/>
       <c r="D122" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="81" t="s">
+      <c r="A123" s="82" t="s">
         <v>472</v>
       </c>
-      <c r="B123" s="81">
+      <c r="B123" s="82">
         <v>348.0</v>
       </c>
-      <c r="C123" s="83"/>
+      <c r="C123" s="84"/>
       <c r="H123" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="81" t="s">
+      <c r="A124" s="82" t="s">
         <v>565</v>
       </c>
-      <c r="B124" s="81">
+      <c r="B124" s="82">
         <v>344.0</v>
       </c>
-      <c r="C124" s="83"/>
+      <c r="C124" s="84"/>
       <c r="D124" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="81" t="s">
+      <c r="A125" s="82" t="s">
         <v>394</v>
       </c>
-      <c r="B125" s="81">
+      <c r="B125" s="82">
         <v>315.0</v>
       </c>
-      <c r="C125" s="83"/>
+      <c r="C125" s="84"/>
       <c r="D125" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="81" t="s">
-        <v>824</v>
-      </c>
-      <c r="B126" s="81">
+      <c r="A126" s="82" t="s">
+        <v>827</v>
+      </c>
+      <c r="B126" s="82">
         <v>309.0</v>
       </c>
-      <c r="C126" s="82" t="s">
+      <c r="C126" s="83" t="s">
         <v>458</v>
       </c>
       <c r="D126" s="3">
@@ -30654,25 +30674,25 @@
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="81" t="s">
+      <c r="A127" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="B127" s="81">
+      <c r="B127" s="82">
         <v>283.0</v>
       </c>
-      <c r="C127" s="83"/>
+      <c r="C127" s="84"/>
       <c r="D127" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="81" t="s">
-        <v>825</v>
-      </c>
-      <c r="B128" s="81">
+      <c r="A128" s="82" t="s">
+        <v>828</v>
+      </c>
+      <c r="B128" s="82">
         <v>279.0</v>
       </c>
-      <c r="C128" s="82" t="s">
+      <c r="C128" s="83" t="s">
         <v>84</v>
       </c>
       <c r="D128" s="3">
@@ -30683,13 +30703,13 @@
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="81" t="s">
+      <c r="A129" s="82" t="s">
         <v>503</v>
       </c>
-      <c r="B129" s="81">
+      <c r="B129" s="82">
         <v>278.0</v>
       </c>
-      <c r="C129" s="83"/>
+      <c r="C129" s="84"/>
       <c r="D129" s="3">
         <v>1.0</v>
       </c>
@@ -30698,13 +30718,13 @@
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="81" t="s">
-        <v>826</v>
-      </c>
-      <c r="B130" s="81">
+      <c r="A130" s="82" t="s">
+        <v>829</v>
+      </c>
+      <c r="B130" s="82">
         <v>276.0</v>
       </c>
-      <c r="C130" s="82" t="s">
+      <c r="C130" s="83" t="s">
         <v>253</v>
       </c>
       <c r="D130" s="3">
@@ -30715,73 +30735,73 @@
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="81" t="s">
+      <c r="A131" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="B131" s="81">
+      <c r="B131" s="82">
         <v>274.0</v>
       </c>
-      <c r="C131" s="83"/>
+      <c r="C131" s="84"/>
       <c r="H131" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="81" t="s">
+      <c r="A132" s="82" t="s">
         <v>785</v>
       </c>
-      <c r="B132" s="81">
+      <c r="B132" s="82">
         <v>264.0</v>
       </c>
-      <c r="C132" s="83"/>
+      <c r="C132" s="84"/>
       <c r="D132" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="81" t="s">
+      <c r="A133" s="82" t="s">
         <v>270</v>
       </c>
-      <c r="B133" s="81">
+      <c r="B133" s="82">
         <v>262.0</v>
       </c>
-      <c r="C133" s="83"/>
+      <c r="C133" s="84"/>
       <c r="H133" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="81" t="s">
-        <v>827</v>
-      </c>
-      <c r="B134" s="81">
+      <c r="A134" s="82" t="s">
+        <v>830</v>
+      </c>
+      <c r="B134" s="82">
         <v>250.0</v>
       </c>
-      <c r="C134" s="83"/>
+      <c r="C134" s="84"/>
       <c r="G134" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="81" t="s">
+      <c r="A135" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="B135" s="81">
+      <c r="B135" s="82">
         <v>247.0</v>
       </c>
-      <c r="C135" s="83"/>
+      <c r="C135" s="84"/>
       <c r="E135" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="81" t="s">
-        <v>828</v>
-      </c>
-      <c r="B136" s="81">
+      <c r="A136" s="82" t="s">
+        <v>831</v>
+      </c>
+      <c r="B136" s="82">
         <v>229.0</v>
       </c>
-      <c r="C136" s="82" t="s">
+      <c r="C136" s="83" t="s">
         <v>619</v>
       </c>
       <c r="D136" s="3">
@@ -30789,25 +30809,25 @@
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="81" t="s">
-        <v>829</v>
-      </c>
-      <c r="B137" s="81">
+      <c r="A137" s="82" t="s">
+        <v>832</v>
+      </c>
+      <c r="B137" s="82">
         <v>226.0</v>
       </c>
-      <c r="C137" s="83"/>
+      <c r="C137" s="84"/>
       <c r="H137" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="81" t="s">
+      <c r="A138" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="B138" s="81">
+      <c r="B138" s="82">
         <v>221.0</v>
       </c>
-      <c r="C138" s="83"/>
+      <c r="C138" s="84"/>
       <c r="D138" s="3">
         <v>1.0</v>
       </c>
@@ -30816,109 +30836,109 @@
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="81" t="s">
+      <c r="A139" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="B139" s="81">
+      <c r="B139" s="82">
         <v>210.0</v>
       </c>
-      <c r="C139" s="83"/>
+      <c r="C139" s="84"/>
       <c r="I139" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="81" t="s">
+      <c r="A140" s="82" t="s">
         <v>456</v>
       </c>
-      <c r="B140" s="81">
+      <c r="B140" s="82">
         <v>209.0</v>
       </c>
-      <c r="C140" s="83"/>
+      <c r="C140" s="84"/>
       <c r="H140" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="81" t="s">
+      <c r="A141" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="B141" s="81">
+      <c r="B141" s="82">
         <v>181.0</v>
       </c>
-      <c r="C141" s="83"/>
+      <c r="C141" s="84"/>
       <c r="H141" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="81" t="s">
+      <c r="A142" s="82" t="s">
         <v>466</v>
       </c>
-      <c r="B142" s="81">
+      <c r="B142" s="82">
         <v>175.0</v>
       </c>
-      <c r="C142" s="83"/>
+      <c r="C142" s="84"/>
       <c r="I142" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="81" t="s">
+      <c r="A143" s="82" t="s">
         <v>597</v>
       </c>
-      <c r="B143" s="81">
+      <c r="B143" s="82">
         <v>151.0</v>
       </c>
-      <c r="C143" s="83"/>
+      <c r="C143" s="84"/>
       <c r="D143" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="81" t="s">
+      <c r="A144" s="82" t="s">
         <v>253</v>
       </c>
-      <c r="B144" s="81">
+      <c r="B144" s="82">
         <v>141.0</v>
       </c>
-      <c r="C144" s="83"/>
+      <c r="C144" s="84"/>
       <c r="D144" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" s="81" t="s">
+      <c r="A145" s="82" t="s">
         <v>439</v>
       </c>
-      <c r="B145" s="81">
+      <c r="B145" s="82">
         <v>128.0</v>
       </c>
-      <c r="C145" s="83"/>
+      <c r="C145" s="84"/>
       <c r="H145" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="81" t="s">
+      <c r="A146" s="82" t="s">
         <v>655</v>
       </c>
-      <c r="B146" s="81">
+      <c r="B146" s="82">
         <v>125.0</v>
       </c>
-      <c r="C146" s="83"/>
+      <c r="C146" s="84"/>
       <c r="H146" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" s="81" t="s">
+      <c r="A147" s="82" t="s">
         <v>658</v>
       </c>
-      <c r="B147" s="81">
+      <c r="B147" s="82">
         <v>90.0</v>
       </c>
-      <c r="C147" s="83"/>
+      <c r="C147" s="84"/>
       <c r="D147" s="3">
         <v>1.0</v>
       </c>
@@ -30927,25 +30947,25 @@
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="81" t="s">
+      <c r="A148" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B148" s="81">
+      <c r="B148" s="82">
         <v>22.0</v>
       </c>
-      <c r="C148" s="83"/>
+      <c r="C148" s="84"/>
       <c r="E148" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="81" t="s">
-        <v>830</v>
-      </c>
-      <c r="B149" s="81">
+      <c r="A149" s="82" t="s">
+        <v>833</v>
+      </c>
+      <c r="B149" s="82">
         <v>26.0</v>
       </c>
-      <c r="C149" s="82" t="s">
+      <c r="C149" s="83" t="s">
         <v>472</v>
       </c>
       <c r="H149" s="3">
@@ -30953,49 +30973,49 @@
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="81" t="s">
+      <c r="A150" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="B150" s="81">
+      <c r="B150" s="82">
         <v>29.0</v>
       </c>
-      <c r="C150" s="83"/>
+      <c r="C150" s="84"/>
       <c r="H150" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="81" t="s">
-        <v>831</v>
-      </c>
-      <c r="B151" s="81">
+      <c r="A151" s="82" t="s">
+        <v>834</v>
+      </c>
+      <c r="B151" s="82">
         <v>34.0</v>
       </c>
-      <c r="C151" s="83"/>
+      <c r="C151" s="84"/>
       <c r="H151" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="81" t="s">
+      <c r="A152" s="82" t="s">
         <v>542</v>
       </c>
-      <c r="B152" s="81">
+      <c r="B152" s="82">
         <v>35.0</v>
       </c>
-      <c r="C152" s="83"/>
+      <c r="C152" s="84"/>
       <c r="E152" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="81" t="s">
+      <c r="A153" s="82" t="s">
         <v>583</v>
       </c>
-      <c r="B153" s="81">
+      <c r="B153" s="82">
         <v>61.0</v>
       </c>
-      <c r="C153" s="83"/>
+      <c r="C153" s="84"/>
       <c r="D153" s="3">
         <v>1.0</v>
       </c>
@@ -31004,77 +31024,77 @@
       </c>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="81" t="s">
+      <c r="A154" s="82" t="s">
         <v>609</v>
       </c>
-      <c r="B154" s="81">
+      <c r="B154" s="82">
         <v>59.0</v>
       </c>
-      <c r="C154" s="83"/>
+      <c r="C154" s="84"/>
       <c r="H154" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="81" t="s">
-        <v>832</v>
-      </c>
-      <c r="B155" s="81">
+      <c r="A155" s="82" t="s">
+        <v>835</v>
+      </c>
+      <c r="B155" s="82">
         <v>74.0</v>
       </c>
-      <c r="C155" s="83"/>
+      <c r="C155" s="84"/>
       <c r="H155" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="81" t="s">
+      <c r="A156" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="B156" s="81">
+      <c r="B156" s="82">
         <v>12.0</v>
       </c>
-      <c r="C156" s="83"/>
+      <c r="C156" s="84"/>
       <c r="H156" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="81" t="s">
+      <c r="A157" s="82" t="s">
         <v>256</v>
       </c>
-      <c r="B157" s="81">
+      <c r="B157" s="82">
         <v>80.0</v>
       </c>
-      <c r="C157" s="83"/>
+      <c r="C157" s="84"/>
       <c r="H157" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="81"/>
-      <c r="B158" s="81"/>
-      <c r="C158" s="83"/>
+      <c r="A158" s="82"/>
+      <c r="B158" s="82"/>
+      <c r="C158" s="84"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="85"/>
-      <c r="B159" s="85"/>
-      <c r="C159" s="83"/>
+      <c r="A159" s="86"/>
+      <c r="B159" s="86"/>
+      <c r="C159" s="84"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="85"/>
-      <c r="B160" s="85"/>
-      <c r="C160" s="83"/>
+      <c r="A160" s="86"/>
+      <c r="B160" s="86"/>
+      <c r="C160" s="84"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" s="85"/>
-      <c r="B161" s="85"/>
-      <c r="C161" s="83"/>
+      <c r="A161" s="86"/>
+      <c r="B161" s="86"/>
+      <c r="C161" s="84"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="85"/>
-      <c r="B162" s="85"/>
-      <c r="C162" s="83"/>
+      <c r="A162" s="86"/>
+      <c r="B162" s="86"/>
+      <c r="C162" s="84"/>
     </row>
     <row r="163" ht="14.25" customHeight="1"/>
     <row r="164" ht="14.25" customHeight="1"/>
@@ -31951,7 +31971,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>11</v>
@@ -32015,7 +32035,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>307</v>
@@ -32026,7 +32046,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>327</v>
@@ -32037,7 +32057,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>307</v>
@@ -32048,7 +32068,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>327</v>
@@ -32083,7 +32103,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
Fixing bug in LVIS COCO converter
</commit_message>
<xml_diff>
--- a/GoogleOpenImages-allClasses.xlsx
+++ b/GoogleOpenImages-allClasses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="843">
   <si>
     <t>class</t>
   </si>
@@ -2482,6 +2482,9 @@
   </si>
   <si>
     <t>chopping board</t>
+  </si>
+  <si>
+    <t>statue (sculpture)</t>
   </si>
   <si>
     <t>bow (decorative ribbons)</t>
@@ -29211,7 +29214,6 @@
         <v>2203.0</v>
       </c>
       <c r="C10" s="85"/>
-      <c r="E10" s="19"/>
       <c r="G10" s="3">
         <v>1.0</v>
       </c>
@@ -30298,12 +30300,14 @@
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="86" t="s">
-        <v>734</v>
+        <v>820</v>
       </c>
       <c r="B97" s="83">
         <v>727.0</v>
       </c>
-      <c r="C97" s="85"/>
+      <c r="C97" s="84" t="s">
+        <v>734</v>
+      </c>
       <c r="E97" s="3">
         <v>1.0</v>
       </c>
@@ -30451,13 +30455,13 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="86" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B109" s="83">
         <v>561.0</v>
       </c>
       <c r="C109" s="84" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D109" s="3">
         <v>1.0</v>
@@ -30468,7 +30472,7 @@
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="83" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B110" s="83">
         <v>546.0</v>
@@ -30480,7 +30484,7 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="83" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B111" s="83">
         <v>502.0</v>
@@ -30518,7 +30522,7 @@
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="83" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B114" s="83">
         <v>432.0</v>
@@ -30532,7 +30536,7 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="83" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B115" s="83">
         <v>424.0</v>
@@ -30560,7 +30564,7 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="86" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B117" s="83">
         <v>405.0</v>
@@ -30613,7 +30617,7 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="83" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B121" s="83">
         <v>359.0</v>
@@ -30673,7 +30677,7 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="83" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B126" s="83">
         <v>309.0</v>
@@ -30699,7 +30703,7 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="83" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B128" s="83">
         <v>279.0</v>
@@ -30732,7 +30736,7 @@
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="83" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B130" s="83">
         <v>276.0</v>
@@ -30785,7 +30789,7 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="83" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B134" s="83">
         <v>250.0</v>
@@ -30809,7 +30813,7 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="83" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B136" s="83">
         <v>229.0</v>
@@ -30973,7 +30977,7 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="83" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B149" s="83">
         <v>26.0</v>
@@ -30999,7 +31003,7 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="83" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B151" s="83">
         <v>34.0</v>
@@ -31050,7 +31054,7 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="83" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B155" s="83">
         <v>74.0</v>
@@ -31984,7 +31988,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>11</v>
@@ -32048,7 +32052,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>307</v>
@@ -32059,7 +32063,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>327</v>
@@ -32070,7 +32074,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>307</v>
@@ -32081,7 +32085,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>327</v>
@@ -32116,7 +32120,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
Updated class for toj
</commit_message>
<xml_diff>
--- a/GoogleOpenImages-allClasses.xlsx
+++ b/GoogleOpenImages-allClasses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="852">
   <si>
     <t>class</t>
   </si>
@@ -2367,6 +2367,12 @@
     <t>doorknob</t>
   </si>
   <si>
+    <t>earring</t>
+  </si>
+  <si>
+    <t>jewelry</t>
+  </si>
+  <si>
     <t>life jacket</t>
   </si>
   <si>
@@ -2391,9 +2397,6 @@
     <t>Toilet</t>
   </si>
   <si>
-    <t>earring</t>
-  </si>
-  <si>
     <t>License plate</t>
   </si>
   <si>
@@ -2421,6 +2424,9 @@
     <t>tank top (clothing)</t>
   </si>
   <si>
+    <t>top</t>
+  </si>
+  <si>
     <t>toilet tissue</t>
   </si>
   <si>
@@ -2436,6 +2442,9 @@
     <t>microwave oven</t>
   </si>
   <si>
+    <t>blouse</t>
+  </si>
+  <si>
     <t>lightbulb</t>
   </si>
   <si>
@@ -2464,9 +2473,6 @@
   </si>
   <si>
     <t>bow (decorative ribbons)</t>
-  </si>
-  <si>
-    <t>bow</t>
   </si>
   <si>
     <t>pot</t>
@@ -2862,7 +2868,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3093,6 +3099,9 @@
     <xf borderId="0" fillId="6" fontId="6" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -3129,6 +3138,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="7" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -4401,9 +4411,6 @@
       <c r="G45" s="3">
         <v>1.0</v>
       </c>
-      <c r="I45" s="3">
-        <v>1.0</v>
-      </c>
       <c r="O45" s="4"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
@@ -15636,7 +15643,7 @@
       </c>
       <c r="I604" s="19">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J604" s="19">
         <f t="shared" si="1"/>
@@ -15655,7 +15662,7 @@
       </c>
       <c r="N604" s="19">
         <f t="shared" ref="N604:N606" si="2">SUM(F604:L604)</f>
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O604" s="11"/>
     </row>
@@ -15709,7 +15716,7 @@
       </c>
       <c r="I606" s="19">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J606" s="19">
         <f t="shared" si="3"/>
@@ -15728,7 +15735,7 @@
       </c>
       <c r="N606" s="19">
         <f t="shared" si="2"/>
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O606" s="11"/>
       <c r="P606" s="22">
@@ -18510,9 +18517,6 @@
       <c r="G45" s="3">
         <v>1.0</v>
       </c>
-      <c r="I45" s="3">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
@@ -18748,7 +18752,9 @@
       <c r="D58" s="1">
         <v>102.0</v>
       </c>
-      <c r="E58" s="1"/>
+      <c r="E58" s="2" t="s">
+        <v>243</v>
+      </c>
       <c r="F58" s="75"/>
       <c r="I58" s="3">
         <v>1.0</v>
@@ -19882,7 +19888,9 @@
       <c r="D118" s="1">
         <v>84.0</v>
       </c>
-      <c r="E118" s="1"/>
+      <c r="E118" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="F118" s="75"/>
       <c r="I118" s="3">
         <v>1.0</v>
@@ -20868,7 +20876,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="75"/>
       <c r="I171" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="172" ht="14.25" customHeight="1">
@@ -21009,7 +21017,9 @@
       <c r="D179" s="1">
         <v>21.0</v>
       </c>
-      <c r="E179" s="1"/>
+      <c r="E179" s="82" t="s">
+        <v>781</v>
+      </c>
       <c r="F179" s="75"/>
       <c r="I179" s="3">
         <v>1.0</v>
@@ -21509,7 +21519,7 @@
       </c>
       <c r="F205" s="75"/>
       <c r="I205" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="206" ht="14.25" customHeight="1">
@@ -22374,9 +22384,6 @@
       <c r="G250" s="3">
         <v>1.0</v>
       </c>
-      <c r="I250" s="3">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="251" ht="14.25" customHeight="1">
       <c r="A251" s="5" t="s">
@@ -22997,7 +23004,7 @@
       <c r="E282" s="1"/>
       <c r="F282" s="75"/>
       <c r="I282" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="283" ht="14.25" customHeight="1">
@@ -23049,7 +23056,9 @@
       <c r="D285" s="1">
         <v>285.0</v>
       </c>
-      <c r="E285" s="1"/>
+      <c r="E285" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="F285" s="75"/>
       <c r="I285" s="3">
         <v>1.0</v>
@@ -23976,7 +23985,9 @@
       <c r="D336" s="1">
         <v>32.0</v>
       </c>
-      <c r="E336" s="1"/>
+      <c r="E336" s="2" t="s">
+        <v>536</v>
+      </c>
       <c r="F336" s="75"/>
       <c r="I336" s="3">
         <v>1.0</v>
@@ -24290,7 +24301,9 @@
       <c r="D353" s="1">
         <v>56.0</v>
       </c>
-      <c r="E353" s="1"/>
+      <c r="E353" s="2" t="s">
+        <v>782</v>
+      </c>
       <c r="F353" s="75"/>
       <c r="I353" s="3">
         <v>1.0</v>
@@ -24884,7 +24897,7 @@
         <v>48.0</v>
       </c>
       <c r="E385" s="3" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="F385" s="75"/>
       <c r="I385" s="3">
@@ -25799,7 +25812,7 @@
         <v>2.0</v>
       </c>
       <c r="E433" s="14" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="F433" s="77"/>
       <c r="J433" s="3">
@@ -25819,7 +25832,9 @@
       <c r="D434" s="1">
         <v>110.0</v>
       </c>
-      <c r="E434" s="1"/>
+      <c r="E434" s="2" t="s">
+        <v>243</v>
+      </c>
       <c r="F434" s="75"/>
       <c r="I434" s="3">
         <v>1.0</v>
@@ -26275,7 +26290,7 @@
       <c r="E458" s="1"/>
       <c r="F458" s="75"/>
       <c r="I458" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="459" ht="14.25" customHeight="1">
@@ -26753,7 +26768,7 @@
       <c r="C484" s="1">
         <v>225.0</v>
       </c>
-      <c r="D484" s="82">
+      <c r="D484" s="83">
         <v>62.0</v>
       </c>
       <c r="E484" s="1"/>
@@ -26813,9 +26828,6 @@
         <v>559</v>
       </c>
       <c r="F487" s="75"/>
-      <c r="I487" s="3">
-        <v>1.0</v>
-      </c>
       <c r="L487" s="3">
         <v>1.0</v>
       </c>
@@ -27200,7 +27212,7 @@
         <v>1.0</v>
       </c>
       <c r="I507" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="508" ht="14.25" customHeight="1">
@@ -27700,9 +27712,6 @@
       </c>
       <c r="E533" s="1"/>
       <c r="F533" s="75"/>
-      <c r="I533" s="3">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="534" ht="14.25" customHeight="1">
       <c r="A534" s="5" t="s">
@@ -28440,10 +28449,9 @@
       </c>
       <c r="E573" s="1"/>
       <c r="F573" s="75"/>
-      <c r="I573" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J573" s="7"/>
+      <c r="J573" s="7">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="574" ht="14.25" customHeight="1">
       <c r="A574" s="5" t="s">
@@ -28994,12 +29002,12 @@
       <c r="F603" s="75"/>
     </row>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="A604" s="83"/>
+      <c r="A604" s="84"/>
       <c r="D604" s="58"/>
       <c r="F604" s="75"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="A605" s="84"/>
+      <c r="A605" s="85"/>
       <c r="D605" s="67"/>
       <c r="F605" s="75"/>
     </row>
@@ -29009,27 +29017,27 @@
       <c r="F606" s="75"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="A607" s="83"/>
+      <c r="A607" s="84"/>
       <c r="D607" s="67"/>
       <c r="F607" s="75"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="A608" s="83"/>
+      <c r="A608" s="84"/>
       <c r="D608" s="63"/>
       <c r="F608" s="75"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="A609" s="83"/>
+      <c r="A609" s="84"/>
       <c r="D609" s="58"/>
       <c r="F609" s="75"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="A610" s="83"/>
+      <c r="A610" s="84"/>
       <c r="D610" s="58"/>
       <c r="F610" s="75"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="A611" s="85"/>
+      <c r="A611" s="86"/>
       <c r="D611" s="58"/>
       <c r="F611" s="75"/>
     </row>
@@ -29039,12 +29047,12 @@
       <c r="F612" s="75"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="A613" s="83"/>
+      <c r="A613" s="84"/>
       <c r="D613" s="63"/>
       <c r="F613" s="75"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="A614" s="86"/>
+      <c r="A614" s="87"/>
       <c r="D614" s="56"/>
       <c r="F614" s="75"/>
     </row>
@@ -29053,32 +29061,32 @@
       <c r="F615" s="75"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="A616" s="86"/>
+      <c r="A616" s="87"/>
       <c r="D616" s="56"/>
       <c r="F616" s="75"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="A617" s="87"/>
+      <c r="A617" s="88"/>
       <c r="D617" s="67"/>
       <c r="F617" s="75"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="A618" s="83"/>
+      <c r="A618" s="84"/>
       <c r="D618" s="67"/>
       <c r="F618" s="75"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="A619" s="83"/>
+      <c r="A619" s="84"/>
       <c r="D619" s="67"/>
       <c r="F619" s="75"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="A620" s="87"/>
+      <c r="A620" s="88"/>
       <c r="D620" s="67"/>
       <c r="F620" s="75"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="A621" s="83"/>
+      <c r="A621" s="84"/>
       <c r="D621" s="62"/>
       <c r="F621" s="75"/>
     </row>
@@ -29097,12 +29105,12 @@
       <c r="F624" s="75"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="A625" s="88"/>
+      <c r="A625" s="89"/>
       <c r="D625" s="58"/>
       <c r="F625" s="75"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="A626" s="89"/>
+      <c r="A626" s="90"/>
       <c r="D626" s="62"/>
       <c r="F626" s="75"/>
     </row>
@@ -29124,18 +29132,18 @@
       <c r="F630" s="75"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="A631" s="85"/>
+      <c r="A631" s="86"/>
       <c r="D631" s="72"/>
       <c r="F631" s="75"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="A632" s="88"/>
-      <c r="D632" s="90"/>
+      <c r="A632" s="89"/>
+      <c r="D632" s="91"/>
       <c r="F632" s="75"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
       <c r="A633" s="71"/>
-      <c r="D633" s="90"/>
+      <c r="D633" s="91"/>
       <c r="F633" s="75"/>
     </row>
     <row r="634" ht="14.25" customHeight="1">
@@ -30295,13 +30303,13 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="91" t="s">
-        <v>783</v>
-      </c>
-      <c r="B2" s="91">
+      <c r="A2" s="92" t="s">
+        <v>785</v>
+      </c>
+      <c r="B2" s="92">
         <v>164.0</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="93" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3">
@@ -30309,13 +30317,13 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="91" t="s">
-        <v>784</v>
-      </c>
-      <c r="B3" s="91">
+      <c r="A3" s="92" t="s">
+        <v>786</v>
+      </c>
+      <c r="B3" s="92">
         <v>2246.0</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="93" t="s">
         <v>482</v>
       </c>
       <c r="J3" s="3">
@@ -30323,90 +30331,90 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="92" t="s">
         <v>549</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="92">
         <v>2231.0</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="94"/>
       <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="92" t="s">
         <v>534</v>
       </c>
-      <c r="B5" s="91">
+      <c r="B5" s="92">
         <v>2216.0</v>
       </c>
-      <c r="C5" s="93"/>
+      <c r="C5" s="94"/>
       <c r="J5" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="95" t="s">
         <v>690</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="92">
         <v>2215.0</v>
       </c>
-      <c r="C6" s="93"/>
+      <c r="C6" s="94"/>
       <c r="J6" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="92">
         <v>2214.0</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="94"/>
       <c r="E7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="95"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="93"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="94"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="92" t="s">
         <v>456</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="92">
         <v>2213.0</v>
       </c>
-      <c r="C9" s="93"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="92">
         <v>2203.0</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="94"/>
       <c r="G10" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="92" t="s">
         <v>641</v>
       </c>
-      <c r="B11" s="91">
+      <c r="B11" s="92">
         <v>2203.0</v>
       </c>
-      <c r="C11" s="93"/>
+      <c r="C11" s="94"/>
       <c r="E11" s="3">
         <v>1.0</v>
       </c>
@@ -30415,25 +30423,25 @@
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="92" t="s">
         <v>658</v>
       </c>
-      <c r="B12" s="91">
+      <c r="B12" s="92">
         <v>2193.0</v>
       </c>
-      <c r="C12" s="93"/>
+      <c r="C12" s="94"/>
       <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="91">
+      <c r="B13" s="92">
         <v>2182.0</v>
       </c>
-      <c r="C13" s="93"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="3">
         <v>1.0</v>
       </c>
@@ -30445,13 +30453,13 @@
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="91" t="s">
-        <v>785</v>
-      </c>
-      <c r="B14" s="91">
+      <c r="A14" s="92" t="s">
+        <v>787</v>
+      </c>
+      <c r="B14" s="92">
         <v>2190.0</v>
       </c>
-      <c r="C14" s="92" t="s">
+      <c r="C14" s="93" t="s">
         <v>172</v>
       </c>
       <c r="D14" s="3">
@@ -30459,13 +30467,13 @@
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="94" t="s">
-        <v>786</v>
-      </c>
-      <c r="B15" s="91">
+      <c r="A15" s="95" t="s">
+        <v>788</v>
+      </c>
+      <c r="B15" s="92">
         <v>2188.0</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="93" t="s">
         <v>152</v>
       </c>
       <c r="D15" s="3">
@@ -30473,98 +30481,97 @@
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="92" t="s">
         <v>243</v>
       </c>
-      <c r="B16" s="91">
+      <c r="B16" s="92">
         <v>2182.0</v>
       </c>
-      <c r="C16" s="93"/>
+      <c r="C16" s="94"/>
       <c r="G16" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="95" t="s">
         <v>699</v>
       </c>
-      <c r="B17" s="91">
+      <c r="B17" s="92">
         <v>2178.0</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="G17" s="3">
-        <v>1.0</v>
-      </c>
+      <c r="C17" s="94"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="92" t="s">
         <v>528</v>
       </c>
-      <c r="B18" s="91">
+      <c r="B18" s="92">
         <v>2174.0</v>
       </c>
-      <c r="C18" s="93"/>
+      <c r="C18" s="94"/>
       <c r="D18" s="19"/>
       <c r="G18" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="91" t="s">
+      <c r="A19" s="92" t="s">
         <v>535</v>
       </c>
-      <c r="B19" s="91">
+      <c r="B19" s="92">
         <v>2171.0</v>
       </c>
-      <c r="C19" s="93"/>
+      <c r="C19" s="94"/>
       <c r="J19" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="92" t="s">
         <v>414</v>
       </c>
-      <c r="B20" s="91">
+      <c r="B20" s="92">
         <v>2167.0</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="93" t="s">
+        <v>782</v>
+      </c>
       <c r="G20" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="91" t="s">
+      <c r="A21" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="91">
+      <c r="B21" s="92">
         <v>2163.0</v>
       </c>
-      <c r="C21" s="93"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="91" t="s">
+      <c r="A22" s="92" t="s">
         <v>460</v>
       </c>
-      <c r="B22" s="91">
+      <c r="B22" s="92">
         <v>2163.0</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="94"/>
       <c r="H22" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="91" t="s">
-        <v>787</v>
-      </c>
-      <c r="B23" s="91">
+      <c r="A23" s="92" t="s">
+        <v>789</v>
+      </c>
+      <c r="B23" s="92">
         <v>2162.0</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="93" t="s">
         <v>598</v>
       </c>
       <c r="D23" s="3">
@@ -30572,25 +30579,25 @@
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="91" t="s">
+      <c r="A24" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="91">
+      <c r="B24" s="92">
         <v>2157.0</v>
       </c>
-      <c r="C24" s="93"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="95" t="s">
         <v>703</v>
       </c>
-      <c r="B25" s="91">
+      <c r="B25" s="92">
         <v>2155.0</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="93" t="s">
         <v>657</v>
       </c>
       <c r="E25" s="3">
@@ -30598,207 +30605,205 @@
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="92" t="s">
         <v>263</v>
       </c>
-      <c r="B26" s="91">
+      <c r="B26" s="92">
         <v>2152.0</v>
       </c>
-      <c r="C26" s="93"/>
+      <c r="C26" s="94"/>
       <c r="G26" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="91" t="s">
-        <v>788</v>
-      </c>
-      <c r="B27" s="91">
+      <c r="A27" s="92" t="s">
+        <v>790</v>
+      </c>
+      <c r="B27" s="92">
         <v>2152.0</v>
       </c>
-      <c r="C27" s="93"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="91" t="s">
+      <c r="A28" s="92" t="s">
         <v>644</v>
       </c>
-      <c r="B28" s="91">
+      <c r="B28" s="92">
         <v>2138.0</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="91" t="s">
+      <c r="A29" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="91">
+      <c r="B29" s="92">
         <v>2140.0</v>
       </c>
-      <c r="C29" s="93"/>
+      <c r="C29" s="94"/>
       <c r="D29" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="91" t="s">
-        <v>789</v>
-      </c>
-      <c r="B30" s="91">
+      <c r="A30" s="92" t="s">
+        <v>781</v>
+      </c>
+      <c r="B30" s="92">
         <v>2133.0</v>
       </c>
-      <c r="C30" s="91" t="s">
-        <v>214</v>
-      </c>
+      <c r="C30" s="97"/>
       <c r="G30" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="91" t="s">
+      <c r="A31" s="92" t="s">
         <v>399</v>
       </c>
-      <c r="B31" s="91">
+      <c r="B31" s="92">
         <v>2132.0</v>
       </c>
-      <c r="C31" s="93"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="94" t="s">
-        <v>790</v>
-      </c>
-      <c r="B32" s="91">
+      <c r="A32" s="95" t="s">
+        <v>791</v>
+      </c>
+      <c r="B32" s="92">
         <v>2129.0</v>
       </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="94"/>
       <c r="E32" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="91" t="s">
+      <c r="A33" s="92" t="s">
         <v>581</v>
       </c>
-      <c r="B33" s="91">
+      <c r="B33" s="92">
         <v>2127.0</v>
       </c>
-      <c r="C33" s="93"/>
+      <c r="C33" s="94"/>
       <c r="J33" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="91" t="s">
+      <c r="A34" s="92" t="s">
         <v>355</v>
       </c>
-      <c r="B34" s="91">
+      <c r="B34" s="92">
         <v>2125.0</v>
       </c>
-      <c r="C34" s="93"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="92" t="s">
         <v>216</v>
       </c>
-      <c r="B35" s="91">
+      <c r="B35" s="92">
         <v>2115.0</v>
       </c>
-      <c r="C35" s="93"/>
+      <c r="C35" s="94"/>
       <c r="I35" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="91" t="s">
+      <c r="A36" s="92" t="s">
         <v>244</v>
       </c>
-      <c r="B36" s="91">
+      <c r="B36" s="92">
         <v>2114.0</v>
       </c>
-      <c r="C36" s="93"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="92" t="s">
         <v>260</v>
       </c>
-      <c r="B37" s="91">
+      <c r="B37" s="92">
         <v>2113.0</v>
       </c>
-      <c r="C37" s="93"/>
+      <c r="C37" s="94"/>
       <c r="I37" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="91">
+      <c r="B38" s="92">
         <v>2106.0</v>
       </c>
-      <c r="C38" s="93"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="94" t="s">
+      <c r="A39" s="95" t="s">
         <v>708</v>
       </c>
-      <c r="B39" s="91">
+      <c r="B39" s="92">
         <v>2088.0</v>
       </c>
-      <c r="C39" s="93"/>
+      <c r="C39" s="94"/>
       <c r="G39" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="92" t="s">
         <v>363</v>
       </c>
-      <c r="B40" s="91">
+      <c r="B40" s="92">
         <v>2067.0</v>
       </c>
-      <c r="C40" s="93"/>
+      <c r="C40" s="94"/>
       <c r="D40" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="91" t="s">
+      <c r="A41" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="91">
+      <c r="B41" s="92">
         <v>1997.0</v>
       </c>
-      <c r="C41" s="93"/>
+      <c r="C41" s="94"/>
       <c r="H41" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="91">
+      <c r="B42" s="92">
         <v>1997.0</v>
       </c>
-      <c r="C42" s="93"/>
+      <c r="C42" s="94"/>
       <c r="D42" s="3">
         <v>1.0</v>
       </c>
@@ -30807,82 +30812,84 @@
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="91" t="s">
-        <v>791</v>
-      </c>
-      <c r="B43" s="91">
+      <c r="A43" s="92" t="s">
+        <v>792</v>
+      </c>
+      <c r="B43" s="92">
         <v>1995.0</v>
       </c>
-      <c r="C43" s="93"/>
+      <c r="C43" s="94"/>
       <c r="J43" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="94" t="s">
+      <c r="A44" s="95" t="s">
         <v>780</v>
       </c>
-      <c r="B44" s="91">
+      <c r="B44" s="92">
         <v>1948.0</v>
       </c>
-      <c r="C44" s="93"/>
+      <c r="C44" s="94"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="91" t="s">
-        <v>792</v>
-      </c>
-      <c r="B45" s="91">
+      <c r="A45" s="92" t="s">
+        <v>793</v>
+      </c>
+      <c r="B45" s="92">
         <v>1920.0</v>
       </c>
-      <c r="C45" s="93"/>
+      <c r="C45" s="94"/>
       <c r="E45" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="91" t="s">
+      <c r="A46" s="92" t="s">
         <v>680</v>
       </c>
-      <c r="B46" s="91">
+      <c r="B46" s="92">
         <v>1902.0</v>
       </c>
-      <c r="C46" s="93"/>
+      <c r="C46" s="94"/>
       <c r="I46" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="94" t="s">
+      <c r="A47" s="95" t="s">
         <v>715</v>
       </c>
-      <c r="B47" s="91">
+      <c r="B47" s="92">
         <v>1877.0</v>
       </c>
-      <c r="C47" s="93"/>
+      <c r="C47" s="93" t="s">
+        <v>782</v>
+      </c>
       <c r="G47" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="91" t="s">
+      <c r="A48" s="92" t="s">
         <v>533</v>
       </c>
-      <c r="B48" s="91">
+      <c r="B48" s="92">
         <v>1869.0</v>
       </c>
-      <c r="C48" s="93"/>
+      <c r="C48" s="94"/>
       <c r="D48" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="91" t="s">
+      <c r="A49" s="92" t="s">
         <v>578</v>
       </c>
-      <c r="B49" s="91">
+      <c r="B49" s="92">
         <v>1831.0</v>
       </c>
-      <c r="C49" s="93"/>
+      <c r="C49" s="94"/>
       <c r="D49" s="3">
         <v>1.0</v>
       </c>
@@ -30891,85 +30898,87 @@
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="94" t="s">
-        <v>793</v>
-      </c>
-      <c r="B50" s="91">
+      <c r="A50" s="95" t="s">
+        <v>794</v>
+      </c>
+      <c r="B50" s="92">
         <v>1784.0</v>
       </c>
-      <c r="C50" s="93"/>
+      <c r="C50" s="15" t="s">
+        <v>782</v>
+      </c>
       <c r="G50" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="91" t="s">
+      <c r="A51" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="91">
+      <c r="B51" s="92">
         <v>1709.0</v>
       </c>
-      <c r="C51" s="93"/>
+      <c r="C51" s="94"/>
       <c r="H51" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="91" t="s">
+      <c r="A52" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="91">
+      <c r="B52" s="92">
         <v>1698.0</v>
       </c>
-      <c r="C52" s="93"/>
+      <c r="C52" s="94"/>
       <c r="D52" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="91" t="s">
+      <c r="A53" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="91">
+      <c r="B53" s="92">
         <v>1664.0</v>
       </c>
-      <c r="C53" s="93"/>
+      <c r="C53" s="94"/>
       <c r="G53" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="91" t="s">
+      <c r="A54" s="92" t="s">
         <v>488</v>
       </c>
-      <c r="B54" s="91">
+      <c r="B54" s="92">
         <v>1655.0</v>
       </c>
-      <c r="C54" s="93"/>
+      <c r="C54" s="94"/>
       <c r="D54" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="91" t="s">
-        <v>794</v>
-      </c>
-      <c r="B55" s="91">
+      <c r="A55" s="92" t="s">
+        <v>795</v>
+      </c>
+      <c r="B55" s="92">
         <v>1640.0</v>
       </c>
-      <c r="C55" s="93"/>
+      <c r="C55" s="94"/>
       <c r="D55" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="94" t="s">
-        <v>795</v>
-      </c>
-      <c r="B56" s="91">
+      <c r="A56" s="95" t="s">
+        <v>796</v>
+      </c>
+      <c r="B56" s="92">
         <v>1639.0</v>
       </c>
-      <c r="C56" s="93"/>
+      <c r="C56" s="94"/>
       <c r="G56" s="3">
         <v>1.0</v>
       </c>
@@ -30978,447 +30987,457 @@
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="91" t="s">
+      <c r="A57" s="92" t="s">
         <v>126</v>
       </c>
-      <c r="B57" s="91">
+      <c r="B57" s="92">
         <v>1611.0</v>
       </c>
-      <c r="C57" s="93"/>
+      <c r="C57" s="94"/>
       <c r="I57" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="91" t="s">
+      <c r="A58" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="91">
+      <c r="B58" s="92">
         <v>1578.0</v>
       </c>
-      <c r="C58" s="93"/>
+      <c r="C58" s="93" t="s">
+        <v>243</v>
+      </c>
       <c r="G58" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="91" t="s">
+      <c r="A59" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="91">
+      <c r="B59" s="92">
         <v>1520.0</v>
       </c>
-      <c r="C59" s="93"/>
+      <c r="C59" s="94"/>
       <c r="H59" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="91" t="s">
-        <v>796</v>
-      </c>
-      <c r="B60" s="91">
+      <c r="A60" s="92" t="s">
+        <v>797</v>
+      </c>
+      <c r="B60" s="92">
         <v>1482.0</v>
       </c>
-      <c r="C60" s="93"/>
+      <c r="C60" s="94"/>
       <c r="J60" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="91" t="s">
-        <v>797</v>
-      </c>
-      <c r="B61" s="91">
+      <c r="A61" s="92" t="s">
+        <v>798</v>
+      </c>
+      <c r="B61" s="92">
         <v>1383.0</v>
       </c>
-      <c r="C61" s="93"/>
+      <c r="C61" s="94"/>
       <c r="H61" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="91" t="s">
+      <c r="A62" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="91">
+      <c r="B62" s="92">
         <v>1382.0</v>
       </c>
-      <c r="C62" s="93"/>
+      <c r="C62" s="94"/>
       <c r="H62" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="91" t="s">
+      <c r="A63" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="91">
+      <c r="B63" s="92">
         <v>1339.0</v>
       </c>
-      <c r="C63" s="93"/>
+      <c r="C63" s="94"/>
       <c r="H63" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="91" t="s">
+      <c r="A64" s="92" t="s">
         <v>556</v>
       </c>
-      <c r="B64" s="91">
+      <c r="B64" s="92">
         <v>1287.0</v>
       </c>
-      <c r="C64" s="93"/>
+      <c r="C64" s="94"/>
       <c r="D64" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="91" t="s">
+      <c r="A65" s="92" t="s">
         <v>490</v>
       </c>
-      <c r="B65" s="91">
+      <c r="B65" s="92">
         <v>1273.0</v>
       </c>
-      <c r="C65" s="93"/>
+      <c r="C65" s="94"/>
       <c r="D65" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="91" t="s">
+      <c r="A66" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="91">
+      <c r="B66" s="92">
         <v>1257.0</v>
       </c>
-      <c r="C66" s="93"/>
+      <c r="C66" s="94"/>
       <c r="D66" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="94" t="s">
+      <c r="A67" s="95" t="s">
         <v>728</v>
       </c>
-      <c r="B67" s="91">
+      <c r="B67" s="92">
         <v>1247.0</v>
       </c>
-      <c r="C67" s="93"/>
+      <c r="C67" s="94"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="96" t="s">
-        <v>798</v>
-      </c>
-      <c r="B68" s="91">
+      <c r="A68" s="98" t="s">
+        <v>799</v>
+      </c>
+      <c r="B68" s="92">
         <v>1227.0</v>
       </c>
-      <c r="C68" s="93"/>
+      <c r="C68" s="93" t="s">
+        <v>800</v>
+      </c>
       <c r="G68" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="91" t="s">
+      <c r="A69" s="92" t="s">
         <v>259</v>
       </c>
-      <c r="B69" s="91">
+      <c r="B69" s="92">
         <v>1170.0</v>
       </c>
-      <c r="C69" s="93"/>
+      <c r="C69" s="94"/>
       <c r="D69" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="91" t="s">
-        <v>799</v>
-      </c>
-      <c r="B70" s="91">
+      <c r="A70" s="92" t="s">
+        <v>801</v>
+      </c>
+      <c r="B70" s="92">
         <v>1164.0</v>
       </c>
-      <c r="C70" s="92" t="s">
+      <c r="C70" s="93" t="s">
+        <v>802</v>
+      </c>
+      <c r="D70" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="95" t="s">
+        <v>733</v>
+      </c>
+      <c r="B71" s="92">
+        <v>1130.0</v>
+      </c>
+      <c r="C71" s="93" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="92" t="s">
+        <v>768</v>
+      </c>
+      <c r="B72" s="92">
+        <v>1129.0</v>
+      </c>
+      <c r="C72" s="94"/>
+      <c r="J72" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="92" t="s">
+        <v>804</v>
+      </c>
+      <c r="B73" s="92">
+        <v>1124.0</v>
+      </c>
+      <c r="C73" s="93" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="B74" s="92">
+        <v>1102.0</v>
+      </c>
+      <c r="C74" s="94"/>
+      <c r="H74" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="75" ht="14.25" customHeight="1">
+      <c r="A75" s="92" t="s">
+        <v>805</v>
+      </c>
+      <c r="B75" s="92">
+        <v>1097.0</v>
+      </c>
+      <c r="C75" s="93" t="s">
+        <v>396</v>
+      </c>
+      <c r="D75" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="95" t="s">
+        <v>734</v>
+      </c>
+      <c r="B76" s="92">
+        <v>1089.0</v>
+      </c>
+      <c r="C76" s="93" t="s">
+        <v>806</v>
+      </c>
+      <c r="G76" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" s="92" t="s">
+        <v>525</v>
+      </c>
+      <c r="B77" s="92">
+        <v>1075.0</v>
+      </c>
+      <c r="C77" s="94"/>
+      <c r="I77" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" s="92" t="s">
+        <v>521</v>
+      </c>
+      <c r="B78" s="92">
+        <v>1033.0</v>
+      </c>
+      <c r="C78" s="94"/>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" s="92" t="s">
+        <v>807</v>
+      </c>
+      <c r="B79" s="92">
+        <v>991.0</v>
+      </c>
+      <c r="C79" s="94"/>
+      <c r="D79" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="A80" s="95" t="s">
+        <v>735</v>
+      </c>
+      <c r="B80" s="92">
+        <v>978.0</v>
+      </c>
+      <c r="C80" s="94"/>
+      <c r="G80" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="A81" s="92" t="s">
+        <v>408</v>
+      </c>
+      <c r="B81" s="92">
+        <v>933.0</v>
+      </c>
+      <c r="C81" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="D81" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25" customHeight="1">
+      <c r="A82" s="92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="92">
+        <v>929.0</v>
+      </c>
+      <c r="C82" s="94"/>
+      <c r="D82" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25" customHeight="1">
+      <c r="A83" s="92" t="s">
+        <v>808</v>
+      </c>
+      <c r="B83" s="92">
+        <v>921.0</v>
+      </c>
+      <c r="C83" s="93" t="s">
+        <v>419</v>
+      </c>
+      <c r="H83" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="92">
+        <v>918.0</v>
+      </c>
+      <c r="C84" s="94"/>
+      <c r="H84" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" s="92" t="s">
+        <v>809</v>
+      </c>
+      <c r="B85" s="92">
+        <v>892.0</v>
+      </c>
+      <c r="C85" s="93" t="s">
+        <v>587</v>
+      </c>
+      <c r="G85" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="A86" s="99" t="s">
+        <v>508</v>
+      </c>
+      <c r="B86" s="92">
+        <v>863.0</v>
+      </c>
+      <c r="C86" s="94"/>
+      <c r="G86" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="A87" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" s="92">
+        <v>831.0</v>
+      </c>
+      <c r="C87" s="93" t="s">
+        <v>341</v>
+      </c>
+      <c r="G87" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="A88" s="92" t="s">
+        <v>621</v>
+      </c>
+      <c r="B88" s="92">
+        <v>831.0</v>
+      </c>
+      <c r="C88" s="94"/>
+      <c r="D88" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25" customHeight="1">
+      <c r="A89" s="92" t="s">
+        <v>509</v>
+      </c>
+      <c r="B89" s="92">
+        <v>804.0</v>
+      </c>
+      <c r="C89" s="94"/>
+      <c r="D89" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25" customHeight="1">
+      <c r="A90" s="95" t="s">
+        <v>736</v>
+      </c>
+      <c r="B90" s="92">
+        <v>801.0</v>
+      </c>
+      <c r="C90" s="94"/>
+    </row>
+    <row r="91" ht="14.25" customHeight="1">
+      <c r="A91" s="92" t="s">
+        <v>424</v>
+      </c>
+      <c r="B91" s="92">
+        <v>776.0</v>
+      </c>
+      <c r="C91" s="94"/>
+      <c r="D91" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="92" ht="14.25" customHeight="1">
+      <c r="A92" s="95" t="s">
+        <v>810</v>
+      </c>
+      <c r="B92" s="92">
+        <v>772.0</v>
+      </c>
+      <c r="C92" s="93" t="s">
         <v>800</v>
       </c>
-      <c r="D70" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="94" t="s">
-        <v>733</v>
-      </c>
-      <c r="B71" s="91">
-        <v>1130.0</v>
-      </c>
-      <c r="C71" s="92" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="91" t="s">
-        <v>768</v>
-      </c>
-      <c r="B72" s="91">
-        <v>1129.0</v>
-      </c>
-      <c r="C72" s="93"/>
-      <c r="J72" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="91" t="s">
-        <v>802</v>
-      </c>
-      <c r="B73" s="91">
-        <v>1124.0</v>
-      </c>
-      <c r="C73" s="92" t="s">
-        <v>503</v>
-      </c>
-      <c r="G73" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="91" t="s">
-        <v>204</v>
-      </c>
-      <c r="B74" s="91">
-        <v>1102.0</v>
-      </c>
-      <c r="C74" s="93"/>
-      <c r="H74" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="91" t="s">
-        <v>803</v>
-      </c>
-      <c r="B75" s="91">
-        <v>1097.0</v>
-      </c>
-      <c r="C75" s="92" t="s">
-        <v>396</v>
-      </c>
-      <c r="D75" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="94" t="s">
-        <v>734</v>
-      </c>
-      <c r="B76" s="91">
-        <v>1089.0</v>
-      </c>
-      <c r="C76" s="93"/>
-      <c r="G76" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="91" t="s">
-        <v>525</v>
-      </c>
-      <c r="B77" s="91">
-        <v>1075.0</v>
-      </c>
-      <c r="C77" s="93"/>
-      <c r="I77" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="91" t="s">
-        <v>521</v>
-      </c>
-      <c r="B78" s="91">
-        <v>1033.0</v>
-      </c>
-      <c r="C78" s="93"/>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="91" t="s">
-        <v>804</v>
-      </c>
-      <c r="B79" s="91">
-        <v>991.0</v>
-      </c>
-      <c r="C79" s="93"/>
-      <c r="D79" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="94" t="s">
-        <v>735</v>
-      </c>
-      <c r="B80" s="91">
-        <v>978.0</v>
-      </c>
-      <c r="C80" s="93"/>
-      <c r="G80" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="91" t="s">
-        <v>408</v>
-      </c>
-      <c r="B81" s="91">
-        <v>933.0</v>
-      </c>
-      <c r="C81" s="92" t="s">
-        <v>152</v>
-      </c>
-      <c r="D81" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="91" t="s">
-        <v>52</v>
-      </c>
-      <c r="B82" s="91">
-        <v>929.0</v>
-      </c>
-      <c r="C82" s="93"/>
-      <c r="D82" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="91" t="s">
-        <v>805</v>
-      </c>
-      <c r="B83" s="91">
-        <v>921.0</v>
-      </c>
-      <c r="C83" s="92" t="s">
-        <v>419</v>
-      </c>
-      <c r="H83" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="B84" s="91">
-        <v>918.0</v>
-      </c>
-      <c r="C84" s="93"/>
-      <c r="H84" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="91" t="s">
-        <v>806</v>
-      </c>
-      <c r="B85" s="91">
-        <v>892.0</v>
-      </c>
-      <c r="C85" s="92" t="s">
-        <v>587</v>
-      </c>
-      <c r="G85" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="97" t="s">
-        <v>508</v>
-      </c>
-      <c r="B86" s="91">
-        <v>863.0</v>
-      </c>
-      <c r="C86" s="93"/>
-      <c r="G86" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="B87" s="91">
-        <v>831.0</v>
-      </c>
-      <c r="C87" s="93"/>
-      <c r="G87" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="91" t="s">
-        <v>621</v>
-      </c>
-      <c r="B88" s="91">
-        <v>831.0</v>
-      </c>
-      <c r="C88" s="93"/>
-      <c r="D88" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="91" t="s">
-        <v>509</v>
-      </c>
-      <c r="B89" s="91">
-        <v>804.0</v>
-      </c>
-      <c r="C89" s="93"/>
-      <c r="D89" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="94" t="s">
-        <v>736</v>
-      </c>
-      <c r="B90" s="91">
-        <v>801.0</v>
-      </c>
-      <c r="C90" s="93"/>
-    </row>
-    <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="91" t="s">
-        <v>424</v>
-      </c>
-      <c r="B91" s="91">
-        <v>776.0</v>
-      </c>
-      <c r="C91" s="93"/>
-      <c r="D91" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="94" t="s">
-        <v>807</v>
-      </c>
-      <c r="B92" s="91">
-        <v>772.0</v>
-      </c>
-      <c r="C92" s="93"/>
       <c r="G92" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="91" t="s">
-        <v>808</v>
-      </c>
-      <c r="B93" s="91">
+      <c r="A93" s="92" t="s">
+        <v>811</v>
+      </c>
+      <c r="B93" s="92">
         <v>770.0</v>
       </c>
-      <c r="C93" s="92" t="s">
+      <c r="C93" s="93" t="s">
         <v>500</v>
       </c>
       <c r="E93" s="19"/>
@@ -31427,37 +31446,37 @@
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="91" t="s">
-        <v>809</v>
-      </c>
-      <c r="B94" s="91">
+      <c r="A94" s="92" t="s">
+        <v>812</v>
+      </c>
+      <c r="B94" s="92">
         <v>739.0</v>
       </c>
-      <c r="C94" s="93"/>
+      <c r="C94" s="94"/>
       <c r="H94" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="91" t="s">
+      <c r="A95" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="B95" s="91">
+      <c r="B95" s="92">
         <v>735.0</v>
       </c>
-      <c r="C95" s="93"/>
+      <c r="C95" s="94"/>
       <c r="I95" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="91" t="s">
-        <v>810</v>
-      </c>
-      <c r="B96" s="91">
+      <c r="A96" s="92" t="s">
+        <v>813</v>
+      </c>
+      <c r="B96" s="92">
         <v>732.0</v>
       </c>
-      <c r="C96" s="92" t="s">
+      <c r="C96" s="93" t="s">
         <v>186</v>
       </c>
       <c r="D96" s="3">
@@ -31465,24 +31484,24 @@
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="94" t="s">
-        <v>811</v>
-      </c>
-      <c r="B97" s="91">
+      <c r="A97" s="95" t="s">
+        <v>814</v>
+      </c>
+      <c r="B97" s="92">
         <v>727.0</v>
       </c>
-      <c r="C97" s="92" t="s">
+      <c r="C97" s="93" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="91" t="s">
+      <c r="A98" s="92" t="s">
         <v>624</v>
       </c>
-      <c r="B98" s="91">
+      <c r="B98" s="92">
         <v>719.0</v>
       </c>
-      <c r="C98" s="93"/>
+      <c r="C98" s="94"/>
       <c r="D98" s="3">
         <v>1.0</v>
       </c>
@@ -31491,13 +31510,13 @@
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="91" t="s">
+      <c r="A99" s="92" t="s">
         <v>360</v>
       </c>
-      <c r="B99" s="91">
+      <c r="B99" s="92">
         <v>710.0</v>
       </c>
-      <c r="C99" s="93"/>
+      <c r="C99" s="94"/>
       <c r="D99" s="3">
         <v>1.0</v>
       </c>
@@ -31506,79 +31525,81 @@
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="94" t="s">
+      <c r="A100" s="95" t="s">
         <v>741</v>
       </c>
-      <c r="B100" s="91">
+      <c r="B100" s="92">
         <v>696.0</v>
       </c>
-      <c r="C100" s="93"/>
+      <c r="C100" s="94"/>
       <c r="H100" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="94" t="s">
+      <c r="A101" s="95" t="s">
         <v>743</v>
       </c>
-      <c r="B101" s="91">
+      <c r="B101" s="92">
         <v>695.0</v>
       </c>
-      <c r="C101" s="93"/>
+      <c r="C101" s="94"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="91" t="s">
+      <c r="A102" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="B102" s="91">
+      <c r="B102" s="92">
         <v>674.0</v>
       </c>
-      <c r="C102" s="93"/>
+      <c r="C102" s="94"/>
       <c r="D102" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="94" t="s">
+      <c r="A103" s="95" t="s">
         <v>745</v>
       </c>
-      <c r="B103" s="91">
+      <c r="B103" s="92">
         <v>653.0</v>
       </c>
-      <c r="C103" s="93"/>
+      <c r="C103" s="93" t="s">
+        <v>175</v>
+      </c>
       <c r="G103" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="91" t="s">
+      <c r="A104" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="B104" s="91">
+      <c r="B104" s="92">
         <v>603.0</v>
       </c>
-      <c r="C104" s="93"/>
+      <c r="C104" s="94"/>
       <c r="D104" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="94" t="s">
+      <c r="A105" s="95" t="s">
         <v>747</v>
       </c>
-      <c r="B105" s="91">
+      <c r="B105" s="92">
         <v>598.0</v>
       </c>
-      <c r="C105" s="93"/>
+      <c r="C105" s="94"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="94" t="s">
-        <v>812</v>
-      </c>
-      <c r="B106" s="91">
+      <c r="A106" s="95" t="s">
+        <v>815</v>
+      </c>
+      <c r="B106" s="92">
         <v>588.0</v>
       </c>
-      <c r="C106" s="92" t="s">
+      <c r="C106" s="93" t="s">
         <v>749</v>
       </c>
       <c r="J106" s="3">
@@ -31586,22 +31607,22 @@
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="96" t="s">
+      <c r="A107" s="98" t="s">
         <v>751</v>
       </c>
-      <c r="B107" s="91">
+      <c r="B107" s="92">
         <v>588.0</v>
       </c>
-      <c r="C107" s="93"/>
+      <c r="C107" s="94"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="94" t="s">
+      <c r="A108" s="95" t="s">
         <v>753</v>
       </c>
-      <c r="B108" s="91">
+      <c r="B108" s="92">
         <v>565.0</v>
       </c>
-      <c r="C108" s="93"/>
+      <c r="C108" s="94"/>
       <c r="G108" s="3">
         <v>1.0</v>
       </c>
@@ -31610,36 +31631,31 @@
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="94" t="s">
-        <v>813</v>
-      </c>
-      <c r="B109" s="91">
+      <c r="A109" s="95" t="s">
+        <v>816</v>
+      </c>
+      <c r="B109" s="92">
         <v>561.0</v>
       </c>
-      <c r="C109" s="92" t="s">
-        <v>814</v>
-      </c>
-      <c r="G109" s="3">
-        <v>1.0</v>
-      </c>
+      <c r="C109" s="93"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="91" t="s">
-        <v>815</v>
-      </c>
-      <c r="B110" s="91">
+      <c r="A110" s="92" t="s">
+        <v>817</v>
+      </c>
+      <c r="B110" s="92">
         <v>546.0</v>
       </c>
-      <c r="C110" s="93"/>
+      <c r="C110" s="94"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="91" t="s">
-        <v>816</v>
-      </c>
-      <c r="B111" s="91">
+      <c r="A111" s="92" t="s">
+        <v>818</v>
+      </c>
+      <c r="B111" s="92">
         <v>502.0</v>
       </c>
-      <c r="C111" s="92" t="s">
+      <c r="C111" s="93" t="s">
         <v>614</v>
       </c>
       <c r="D111" s="3">
@@ -31647,31 +31663,31 @@
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="97" t="s">
+      <c r="A112" s="99" t="s">
         <v>758</v>
       </c>
-      <c r="B112" s="91">
+      <c r="B112" s="92">
         <v>480.0</v>
       </c>
-      <c r="C112" s="93"/>
+      <c r="C112" s="94"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="91" t="s">
+      <c r="A113" s="92" t="s">
         <v>410</v>
       </c>
-      <c r="B113" s="91">
+      <c r="B113" s="92">
         <v>473.0</v>
       </c>
-      <c r="C113" s="93"/>
+      <c r="C113" s="94"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="91" t="s">
-        <v>817</v>
-      </c>
-      <c r="B114" s="91">
+      <c r="A114" s="92" t="s">
+        <v>819</v>
+      </c>
+      <c r="B114" s="92">
         <v>432.0</v>
       </c>
-      <c r="C114" s="92" t="s">
+      <c r="C114" s="93" t="s">
         <v>531</v>
       </c>
       <c r="D114" s="3">
@@ -31679,13 +31695,13 @@
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="91" t="s">
-        <v>818</v>
-      </c>
-      <c r="B115" s="91">
+      <c r="A115" s="92" t="s">
+        <v>820</v>
+      </c>
+      <c r="B115" s="92">
         <v>424.0</v>
       </c>
-      <c r="C115" s="92" t="s">
+      <c r="C115" s="93" t="s">
         <v>184</v>
       </c>
       <c r="D115" s="3">
@@ -31693,24 +31709,24 @@
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="91" t="s">
+      <c r="A116" s="92" t="s">
         <v>502</v>
       </c>
-      <c r="B116" s="91">
+      <c r="B116" s="92">
         <v>418.0</v>
       </c>
-      <c r="C116" s="92" t="s">
-        <v>782</v>
+      <c r="C116" s="93" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="94" t="s">
-        <v>819</v>
-      </c>
-      <c r="B117" s="91">
+      <c r="A117" s="95" t="s">
+        <v>821</v>
+      </c>
+      <c r="B117" s="92">
         <v>405.0</v>
       </c>
-      <c r="C117" s="92" t="s">
+      <c r="C117" s="93" t="s">
         <v>624</v>
       </c>
       <c r="D117" s="3">
@@ -31721,82 +31737,82 @@
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="91" t="s">
+      <c r="A118" s="92" t="s">
         <v>368</v>
       </c>
-      <c r="B118" s="91">
+      <c r="B118" s="92">
         <v>393.0</v>
       </c>
-      <c r="C118" s="93"/>
+      <c r="C118" s="94"/>
       <c r="H118" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="91" t="s">
+      <c r="A119" s="92" t="s">
         <v>441</v>
       </c>
-      <c r="B119" s="91">
+      <c r="B119" s="92">
         <v>382.0</v>
       </c>
-      <c r="C119" s="93"/>
+      <c r="C119" s="94"/>
       <c r="D119" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="91" t="s">
+      <c r="A120" s="92" t="s">
         <v>570</v>
       </c>
-      <c r="B120" s="91">
+      <c r="B120" s="92">
         <v>379.0</v>
       </c>
-      <c r="C120" s="93"/>
+      <c r="C120" s="94"/>
       <c r="H120" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="91" t="s">
-        <v>820</v>
-      </c>
-      <c r="B121" s="91">
+      <c r="A121" s="92" t="s">
+        <v>822</v>
+      </c>
+      <c r="B121" s="92">
         <v>359.0</v>
       </c>
-      <c r="C121" s="93"/>
+      <c r="C121" s="94"/>
       <c r="H121" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="91" t="s">
+      <c r="A122" s="92" t="s">
         <v>553</v>
       </c>
-      <c r="B122" s="91">
+      <c r="B122" s="92">
         <v>353.0</v>
       </c>
-      <c r="C122" s="93"/>
+      <c r="C122" s="94"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="91" t="s">
+      <c r="A123" s="92" t="s">
         <v>473</v>
       </c>
-      <c r="B123" s="91">
+      <c r="B123" s="92">
         <v>348.0</v>
       </c>
-      <c r="C123" s="93"/>
+      <c r="C123" s="94"/>
       <c r="H123" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="91" t="s">
+      <c r="A124" s="92" t="s">
         <v>568</v>
       </c>
-      <c r="B124" s="91">
+      <c r="B124" s="92">
         <v>344.0</v>
       </c>
-      <c r="C124" s="92" t="s">
+      <c r="C124" s="93" t="s">
         <v>132</v>
       </c>
       <c r="D124" s="3">
@@ -31804,25 +31820,25 @@
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="91" t="s">
+      <c r="A125" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="B125" s="91">
+      <c r="B125" s="92">
         <v>315.0</v>
       </c>
-      <c r="C125" s="93"/>
+      <c r="C125" s="94"/>
       <c r="D125" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="91" t="s">
-        <v>821</v>
-      </c>
-      <c r="B126" s="91">
+      <c r="A126" s="92" t="s">
+        <v>823</v>
+      </c>
+      <c r="B126" s="92">
         <v>309.0</v>
       </c>
-      <c r="C126" s="92" t="s">
+      <c r="C126" s="93" t="s">
         <v>459</v>
       </c>
       <c r="D126" s="3">
@@ -31830,25 +31846,25 @@
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="91" t="s">
+      <c r="A127" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="B127" s="91">
+      <c r="B127" s="92">
         <v>283.0</v>
       </c>
-      <c r="C127" s="93"/>
+      <c r="C127" s="94"/>
       <c r="D127" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="91" t="s">
-        <v>822</v>
-      </c>
-      <c r="B128" s="91">
+      <c r="A128" s="92" t="s">
+        <v>824</v>
+      </c>
+      <c r="B128" s="92">
         <v>279.0</v>
       </c>
-      <c r="C128" s="92" t="s">
+      <c r="C128" s="93" t="s">
         <v>85</v>
       </c>
       <c r="D128" s="3">
@@ -31860,22 +31876,22 @@
       <c r="I128" s="19"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="91" t="s">
+      <c r="A129" s="92" t="s">
         <v>505</v>
       </c>
-      <c r="B129" s="91">
+      <c r="B129" s="92">
         <v>278.0</v>
       </c>
-      <c r="C129" s="93"/>
+      <c r="C129" s="94"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="91" t="s">
-        <v>823</v>
-      </c>
-      <c r="B130" s="91">
+      <c r="A130" s="92" t="s">
+        <v>825</v>
+      </c>
+      <c r="B130" s="92">
         <v>276.0</v>
       </c>
-      <c r="C130" s="92" t="s">
+      <c r="C130" s="93" t="s">
         <v>254</v>
       </c>
       <c r="D130" s="3">
@@ -31883,61 +31899,61 @@
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="91" t="s">
+      <c r="A131" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="B131" s="91">
+      <c r="B131" s="92">
         <v>274.0</v>
       </c>
-      <c r="C131" s="93"/>
+      <c r="C131" s="94"/>
       <c r="H131" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="91" t="s">
-        <v>824</v>
-      </c>
-      <c r="B132" s="91">
+      <c r="A132" s="92" t="s">
+        <v>826</v>
+      </c>
+      <c r="B132" s="92">
         <v>264.0</v>
       </c>
-      <c r="C132" s="93"/>
+      <c r="C132" s="94"/>
       <c r="D132" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="91" t="s">
+      <c r="A133" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="B133" s="91">
+      <c r="B133" s="92">
         <v>262.0</v>
       </c>
-      <c r="C133" s="93"/>
+      <c r="C133" s="94"/>
       <c r="H133" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="91" t="s">
-        <v>781</v>
-      </c>
-      <c r="B134" s="91">
+      <c r="A134" s="92" t="s">
+        <v>783</v>
+      </c>
+      <c r="B134" s="92">
         <v>250.0</v>
       </c>
-      <c r="C134" s="93"/>
+      <c r="C134" s="94"/>
       <c r="G134" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="91" t="s">
+      <c r="A135" s="92" t="s">
         <v>142</v>
       </c>
-      <c r="B135" s="91">
+      <c r="B135" s="92">
         <v>247.0</v>
       </c>
-      <c r="C135" s="93"/>
+      <c r="C135" s="94"/>
       <c r="D135" s="3">
         <v>1.0</v>
       </c>
@@ -31946,13 +31962,13 @@
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="91" t="s">
-        <v>825</v>
-      </c>
-      <c r="B136" s="91">
+      <c r="A136" s="92" t="s">
+        <v>827</v>
+      </c>
+      <c r="B136" s="92">
         <v>229.0</v>
       </c>
-      <c r="C136" s="92" t="s">
+      <c r="C136" s="93" t="s">
         <v>624</v>
       </c>
       <c r="D136" s="3">
@@ -31960,133 +31976,133 @@
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="91" t="s">
-        <v>826</v>
-      </c>
-      <c r="B137" s="91">
+      <c r="A137" s="92" t="s">
+        <v>828</v>
+      </c>
+      <c r="B137" s="92">
         <v>226.0</v>
       </c>
-      <c r="C137" s="93"/>
+      <c r="C137" s="94"/>
       <c r="H137" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="91" t="s">
+      <c r="A138" s="92" t="s">
         <v>275</v>
       </c>
-      <c r="B138" s="91">
+      <c r="B138" s="92">
         <v>221.0</v>
       </c>
-      <c r="C138" s="93"/>
+      <c r="C138" s="94"/>
       <c r="D138" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="91" t="s">
+      <c r="A139" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="B139" s="91">
+      <c r="B139" s="92">
         <v>210.0</v>
       </c>
-      <c r="C139" s="93"/>
+      <c r="C139" s="94"/>
       <c r="I139" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="91" t="s">
+      <c r="A140" s="92" t="s">
         <v>457</v>
       </c>
-      <c r="B140" s="91">
+      <c r="B140" s="92">
         <v>209.0</v>
       </c>
-      <c r="C140" s="93"/>
+      <c r="C140" s="94"/>
       <c r="H140" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="91" t="s">
+      <c r="A141" s="92" t="s">
         <v>168</v>
       </c>
-      <c r="B141" s="91">
+      <c r="B141" s="92">
         <v>181.0</v>
       </c>
-      <c r="C141" s="93"/>
+      <c r="C141" s="94"/>
       <c r="H141" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="91" t="s">
+      <c r="A142" s="92" t="s">
         <v>467</v>
       </c>
-      <c r="B142" s="91">
+      <c r="B142" s="92">
         <v>175.0</v>
       </c>
-      <c r="C142" s="93"/>
+      <c r="C142" s="94"/>
       <c r="I142" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="91" t="s">
+      <c r="A143" s="92" t="s">
         <v>602</v>
       </c>
-      <c r="B143" s="91">
+      <c r="B143" s="92">
         <v>151.0</v>
       </c>
-      <c r="C143" s="93"/>
+      <c r="C143" s="94"/>
       <c r="D143" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="91" t="s">
+      <c r="A144" s="92" t="s">
         <v>254</v>
       </c>
-      <c r="B144" s="91">
+      <c r="B144" s="92">
         <v>141.0</v>
       </c>
-      <c r="C144" s="93"/>
+      <c r="C144" s="94"/>
       <c r="D144" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" s="91" t="s">
+      <c r="A145" s="92" t="s">
         <v>440</v>
       </c>
-      <c r="B145" s="91">
+      <c r="B145" s="92">
         <v>128.0</v>
       </c>
-      <c r="C145" s="93"/>
+      <c r="C145" s="94"/>
       <c r="H145" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="91" t="s">
+      <c r="A146" s="92" t="s">
         <v>660</v>
       </c>
-      <c r="B146" s="91">
+      <c r="B146" s="92">
         <v>125.0</v>
       </c>
-      <c r="C146" s="93"/>
+      <c r="C146" s="94"/>
       <c r="H146" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" s="91" t="s">
+      <c r="A147" s="92" t="s">
         <v>663</v>
       </c>
-      <c r="B147" s="91">
+      <c r="B147" s="92">
         <v>90.0</v>
       </c>
-      <c r="C147" s="93"/>
+      <c r="C147" s="94"/>
       <c r="D147" s="3">
         <v>1.0</v>
       </c>
@@ -32095,25 +32111,25 @@
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="91" t="s">
+      <c r="A148" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="B148" s="91">
+      <c r="B148" s="92">
         <v>22.0</v>
       </c>
-      <c r="C148" s="93"/>
+      <c r="C148" s="94"/>
       <c r="E148" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="91" t="s">
-        <v>827</v>
-      </c>
-      <c r="B149" s="91">
+      <c r="A149" s="92" t="s">
+        <v>829</v>
+      </c>
+      <c r="B149" s="92">
         <v>26.0</v>
       </c>
-      <c r="C149" s="92" t="s">
+      <c r="C149" s="93" t="s">
         <v>473</v>
       </c>
       <c r="H149" s="3">
@@ -32121,122 +32137,122 @@
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="91" t="s">
+      <c r="A150" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="B150" s="91">
+      <c r="B150" s="92">
         <v>29.0</v>
       </c>
-      <c r="C150" s="93"/>
+      <c r="C150" s="94"/>
       <c r="H150" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="91" t="s">
-        <v>828</v>
-      </c>
-      <c r="B151" s="91">
+      <c r="A151" s="92" t="s">
+        <v>830</v>
+      </c>
+      <c r="B151" s="92">
         <v>34.0</v>
       </c>
-      <c r="C151" s="93"/>
+      <c r="C151" s="94"/>
       <c r="H151" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="91" t="s">
+      <c r="A152" s="92" t="s">
         <v>545</v>
       </c>
-      <c r="B152" s="91">
+      <c r="B152" s="92">
         <v>35.0</v>
       </c>
-      <c r="C152" s="93"/>
+      <c r="C152" s="94"/>
       <c r="E152" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="91" t="s">
+      <c r="A153" s="92" t="s">
         <v>588</v>
       </c>
-      <c r="B153" s="91">
+      <c r="B153" s="92">
         <v>61.0</v>
       </c>
-      <c r="C153" s="93"/>
+      <c r="C153" s="94"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="91" t="s">
+      <c r="A154" s="92" t="s">
         <v>614</v>
       </c>
-      <c r="B154" s="91">
+      <c r="B154" s="92">
         <v>59.0</v>
       </c>
-      <c r="C154" s="92"/>
+      <c r="C154" s="93"/>
       <c r="H154" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="91" t="s">
-        <v>829</v>
-      </c>
-      <c r="B155" s="91">
+      <c r="A155" s="92" t="s">
+        <v>831</v>
+      </c>
+      <c r="B155" s="92">
         <v>74.0</v>
       </c>
-      <c r="C155" s="93"/>
+      <c r="C155" s="94"/>
       <c r="H155" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="91" t="s">
+      <c r="A156" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="B156" s="91">
+      <c r="B156" s="92">
         <v>12.0</v>
       </c>
-      <c r="C156" s="93"/>
+      <c r="C156" s="94"/>
       <c r="H156" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="91" t="s">
+      <c r="A157" s="92" t="s">
         <v>257</v>
       </c>
-      <c r="B157" s="91">
+      <c r="B157" s="92">
         <v>80.0</v>
       </c>
-      <c r="C157" s="93"/>
+      <c r="C157" s="94"/>
       <c r="H157" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="91"/>
-      <c r="B158" s="91"/>
-      <c r="C158" s="93"/>
+      <c r="A158" s="92"/>
+      <c r="B158" s="92"/>
+      <c r="C158" s="94"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="95"/>
-      <c r="B159" s="95"/>
-      <c r="C159" s="93"/>
+      <c r="A159" s="96"/>
+      <c r="B159" s="96"/>
+      <c r="C159" s="94"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="95"/>
-      <c r="B160" s="95"/>
-      <c r="C160" s="93"/>
+      <c r="A160" s="96"/>
+      <c r="B160" s="96"/>
+      <c r="C160" s="94"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" s="95"/>
-      <c r="B161" s="95"/>
-      <c r="C161" s="93"/>
+      <c r="A161" s="96"/>
+      <c r="B161" s="96"/>
+      <c r="C161" s="94"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="95"/>
-      <c r="B162" s="95"/>
-      <c r="C162" s="93"/>
+      <c r="A162" s="96"/>
+      <c r="B162" s="96"/>
+      <c r="C162" s="94"/>
     </row>
     <row r="163" ht="14.25" customHeight="1"/>
     <row r="164" ht="14.25" customHeight="1"/>
@@ -33113,7 +33129,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>11</v>
@@ -33137,7 +33153,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>314</v>
@@ -33148,7 +33164,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>314</v>
@@ -33159,7 +33175,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>316</v>
@@ -33170,7 +33186,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>316</v>
@@ -33181,7 +33197,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>760</v>
@@ -33192,7 +33208,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>760</v>
@@ -33203,7 +33219,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>320</v>
@@ -33214,7 +33230,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>320</v>
@@ -33225,7 +33241,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>324</v>
@@ -33236,7 +33252,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>324</v>
@@ -33247,7 +33263,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>308</v>
@@ -33258,7 +33274,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>308</v>
@@ -33269,7 +33285,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>328</v>
@@ -33280,7 +33296,7 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>328</v>
@@ -33291,7 +33307,7 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>328</v>
@@ -33302,7 +33318,7 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>328</v>
@@ -33313,7 +33329,7 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>308</v>
@@ -33324,7 +33340,7 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>308</v>
@@ -33359,7 +33375,7 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>312</v>

</xml_diff>